<commit_message>
update for FY23-FY27 plan
</commit_message>
<xml_diff>
--- a/data/01_raw/historical/BIRT-splits.xlsx
+++ b/data/01_raw/historical/BIRT-splits.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicholashand/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicholashand/LocalWork/Analysis/five-year-plan-analysis/data/01_raw/historical/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{42688868-2E2A-264E-ABBD-1698B5A533BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CF35DA1-CBB0-1E4E-942C-7F0C7271230E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1580" yWindow="2000" windowWidth="26840" windowHeight="15440" xr2:uid="{1580F8C4-AF3E-5F4A-A010-F100369F5510}"/>
+    <workbookView xWindow="7840" yWindow="2100" windowWidth="26840" windowHeight="15440" activeTab="1" xr2:uid="{1580F8C4-AF3E-5F4A-A010-F100369F5510}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'BIRT History'!$A$1:$AD$31</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,6 +31,7 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t>FY21</t>
   </si>
@@ -181,9 +182,6 @@
     <t>Actual</t>
   </si>
   <si>
-    <t>Projected</t>
-  </si>
-  <si>
     <t>net_income_fraction</t>
   </si>
 </sst>
@@ -194,9 +192,9 @@
   <numFmts count="5">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.0000%"/>
-    <numFmt numFmtId="166" formatCode="0.0%"/>
-    <numFmt numFmtId="167" formatCode="0.0000"/>
-    <numFmt numFmtId="168" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="0.0%"/>
+    <numFmt numFmtId="166" formatCode="0.0000"/>
+    <numFmt numFmtId="167" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="11" x14ac:knownFonts="1">
     <font>
@@ -267,7 +265,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -280,34 +278,13 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="5">
+  <borders count="4">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -354,7 +331,7 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
@@ -390,23 +367,23 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="10" fontId="5" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="10" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="3" fontId="3" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="10" fontId="3" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="3" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="5" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -428,44 +405,43 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="37" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="37" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="37" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="10" fillId="0" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="10" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="10" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="7" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="10" fontId="5" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="5" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="3" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="3" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="3" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="10" fontId="3" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="3" fontId="7" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="37" fontId="7" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="168" fontId="10" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="10" fillId="0" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="10" fillId="0" borderId="4" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="37" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma 2" xfId="3" xr:uid="{C68451E4-A945-6545-A9E6-7D1F8818D189}"/>
@@ -783,10 +759,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A109B183-BE6E-194B-93C2-5208D89F22E1}">
-  <dimension ref="A1:B27"/>
+  <dimension ref="A1:B28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -796,7 +772,7 @@
         <v>45</v>
       </c>
       <c r="B1" s="39" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -1030,6 +1006,14 @@
       </c>
       <c r="B27">
         <f>'BIRT History'!F29</f>
+        <v>0.73</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>2022</v>
+      </c>
+      <c r="B28">
         <v>0.73</v>
       </c>
     </row>
@@ -1043,10 +1027,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AA121"/>
+  <dimension ref="A1:AA122"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="W13" sqref="W13"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1551,9 +1535,9 @@
       <c r="R3" s="27"/>
       <c r="S3" s="27"/>
       <c r="T3" s="27"/>
-      <c r="U3" s="43"/>
-      <c r="V3" s="43"/>
-      <c r="W3" s="43"/>
+      <c r="U3" s="47"/>
+      <c r="V3" s="47"/>
+      <c r="W3" s="47"/>
       <c r="X3" s="25"/>
       <c r="Y3" s="42"/>
     </row>
@@ -1576,31 +1560,31 @@
         <v>0.31</v>
       </c>
       <c r="H4" s="16">
-        <f>G4*R4</f>
+        <f t="shared" ref="H4:H29" si="0">G4*R4</f>
         <v>0</v>
       </c>
       <c r="I4" s="16" t="e">
-        <f>(H4/(1-$L4))-H4</f>
+        <f t="shared" ref="I4:I29" si="1">(H4/(1-$L4))-H4</f>
         <v>#DIV/0!</v>
       </c>
       <c r="J4" s="16">
-        <f>F4*R4</f>
+        <f t="shared" ref="J4:J29" si="2">F4*R4</f>
         <v>0</v>
       </c>
       <c r="K4" s="16" t="e">
-        <f>(J4/(1-$L4))-J4</f>
+        <f t="shared" ref="K4:K29" si="3">(J4/(1-$L4))-J4</f>
         <v>#DIV/0!</v>
       </c>
       <c r="L4" s="18" t="e">
-        <f>S4/(R4+S4)</f>
+        <f t="shared" ref="L4:L29" si="4">S4/(R4+S4)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M4" s="17" t="e">
-        <f>(O4/O3)-1</f>
+        <f t="shared" ref="M4:M29" si="5">(O4/O3)-1</f>
         <v>#DIV/0!</v>
       </c>
       <c r="N4" s="17" t="e">
-        <f>(P4/P3)-1</f>
+        <f t="shared" ref="N4:N29" si="6">(P4/P3)-1</f>
         <v>#DIV/0!</v>
       </c>
       <c r="O4" s="16">
@@ -1615,10 +1599,10 @@
       <c r="R4" s="14"/>
       <c r="S4" s="14"/>
       <c r="T4" s="14">
-        <f>R4+S4</f>
+        <f t="shared" ref="T4:T29" si="7">R4+S4</f>
         <v>0</v>
       </c>
-      <c r="U4" s="59" t="s">
+      <c r="U4" s="48" t="s">
         <v>46</v>
       </c>
       <c r="V4" s="25"/>
@@ -1645,31 +1629,31 @@
         <v>0.31</v>
       </c>
       <c r="H5" s="16">
-        <f>G5*R5</f>
+        <f t="shared" si="0"/>
         <v>66519.490000000005</v>
       </c>
       <c r="I5" s="16">
-        <f>(H5/(1-$L5))-H5</f>
+        <f t="shared" si="1"/>
         <v>9276.4400000000023</v>
       </c>
       <c r="J5" s="16">
-        <f>F5*R5</f>
+        <f t="shared" si="2"/>
         <v>148059.50999999998</v>
       </c>
       <c r="K5" s="16">
-        <f>(J5/(1-$L5))-J5</f>
+        <f t="shared" si="3"/>
         <v>20647.559999999998</v>
       </c>
       <c r="L5" s="18">
-        <f>S5/(R5+S5)</f>
+        <f t="shared" si="4"/>
         <v>0.12238704637570909</v>
       </c>
       <c r="M5" s="17" t="e">
-        <f>(O5/O4)-1</f>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
       <c r="N5" s="17" t="e">
-        <f>(P5/P4)-1</f>
+        <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O5" s="16">
@@ -1688,10 +1672,10 @@
         <v>29924</v>
       </c>
       <c r="T5" s="14">
-        <f>R5+S5</f>
+        <f t="shared" si="7"/>
         <v>244503</v>
       </c>
-      <c r="U5" s="60"/>
+      <c r="U5" s="49"/>
       <c r="V5" s="25"/>
       <c r="W5" s="25"/>
       <c r="X5" s="25"/>
@@ -1716,31 +1700,31 @@
         <v>0.31</v>
       </c>
       <c r="H6" s="16">
-        <f>G6*R6</f>
+        <f t="shared" si="0"/>
         <v>65292.2</v>
       </c>
       <c r="I6" s="16">
-        <f>(H6/(1-$L6))-H6</f>
+        <f t="shared" si="1"/>
         <v>11225.410000000003</v>
       </c>
       <c r="J6" s="16">
-        <f>F6*R6</f>
+        <f t="shared" si="2"/>
         <v>145327.79999999999</v>
       </c>
       <c r="K6" s="16">
-        <f>(J6/(1-$L6))-J6</f>
+        <f t="shared" si="3"/>
         <v>24985.589999999997</v>
       </c>
       <c r="L6" s="18">
-        <f>S6/(R6+S6)</f>
+        <f t="shared" si="4"/>
         <v>0.1467036150240448</v>
       </c>
       <c r="M6" s="17">
-        <f>(O6/O5)-1</f>
+        <f t="shared" si="5"/>
         <v>6.3345745234466788E-2</v>
       </c>
       <c r="N6" s="17">
-        <f>(P6/P5)-1</f>
+        <f t="shared" si="6"/>
         <v>-1.845008132203052E-2</v>
       </c>
       <c r="O6" s="16">
@@ -1759,10 +1743,10 @@
         <v>36211</v>
       </c>
       <c r="T6" s="14">
-        <f>R6+S6</f>
+        <f t="shared" si="7"/>
         <v>246831</v>
       </c>
-      <c r="U6" s="60"/>
+      <c r="U6" s="49"/>
       <c r="V6" s="25"/>
       <c r="W6" s="25"/>
       <c r="X6" s="25"/>
@@ -1787,39 +1771,39 @@
         <v>0.31</v>
       </c>
       <c r="H7" s="16">
-        <f>G7*R7</f>
+        <f t="shared" si="0"/>
         <v>66351.16</v>
       </c>
       <c r="I7" s="16">
-        <f>(H7/(1-$L7))-H7</f>
+        <f t="shared" si="1"/>
         <v>7239.7400000000052</v>
       </c>
       <c r="J7" s="16">
-        <f>F7*R7</f>
+        <f t="shared" si="2"/>
         <v>147684.84</v>
       </c>
       <c r="K7" s="16">
-        <f>(J7/(1-$L7))-J7</f>
+        <f t="shared" si="3"/>
         <v>16114.260000000009</v>
       </c>
       <c r="L7" s="18">
-        <f>S7/(R7+S7)</f>
+        <f t="shared" si="4"/>
         <v>9.8378196217195332E-2</v>
       </c>
       <c r="M7" s="17">
-        <f>(O7/O6)-1</f>
+        <f t="shared" si="5"/>
         <v>3.3442829805143681E-2</v>
       </c>
       <c r="N7" s="17">
-        <f>(P7/P6)-1</f>
+        <f t="shared" si="6"/>
         <v>1.6218782641724605E-2</v>
       </c>
       <c r="O7" s="16">
-        <f>H7/B7</f>
+        <f t="shared" ref="O7:O29" si="8">H7/B7</f>
         <v>224919.18644067799</v>
       </c>
       <c r="P7" s="16">
-        <f>J7/D7</f>
+        <f t="shared" ref="P7:P29" si="9">J7/D7</f>
         <v>2272074.4615384615</v>
       </c>
       <c r="Q7" s="15"/>
@@ -1830,10 +1814,10 @@
         <v>23354</v>
       </c>
       <c r="T7" s="14">
-        <f>R7+S7</f>
+        <f t="shared" si="7"/>
         <v>237390</v>
       </c>
-      <c r="U7" s="60"/>
+      <c r="U7" s="49"/>
       <c r="V7" s="25"/>
       <c r="W7" s="25"/>
       <c r="X7" s="25"/>
@@ -1858,39 +1842,39 @@
         <v>0.31</v>
       </c>
       <c r="H8" s="16">
-        <f>G8*R8</f>
+        <f t="shared" si="0"/>
         <v>72497.22</v>
       </c>
       <c r="I8" s="16">
-        <f>(H8/(1-$L8))-H8</f>
+        <f t="shared" si="1"/>
         <v>6405.2200000000012</v>
       </c>
       <c r="J8" s="16">
-        <f>F8*R8</f>
+        <f t="shared" si="2"/>
         <v>161364.78</v>
       </c>
       <c r="K8" s="16">
-        <f>(J8/(1-$L8))-J8</f>
+        <f t="shared" si="3"/>
         <v>14256.779999999999</v>
       </c>
       <c r="L8" s="18">
-        <f>S8/(R8+S8)</f>
+        <f t="shared" si="4"/>
         <v>8.1178985085885808E-2</v>
       </c>
       <c r="M8" s="17">
-        <f>(O8/O7)-1</f>
+        <f t="shared" si="5"/>
         <v>0.12113264976960392</v>
       </c>
       <c r="N8" s="17">
-        <f>(P8/P7)-1</f>
+        <f t="shared" si="6"/>
         <v>9.2629277317834324E-2</v>
       </c>
       <c r="O8" s="16">
-        <f>H8/B8</f>
+        <f t="shared" si="8"/>
         <v>252164.24347826091</v>
       </c>
       <c r="P8" s="16">
-        <f>J8/D8</f>
+        <f t="shared" si="9"/>
         <v>2482535.076923077</v>
       </c>
       <c r="Q8" s="15"/>
@@ -1901,10 +1885,10 @@
         <v>20662</v>
       </c>
       <c r="T8" s="14">
-        <f>R8+S8</f>
+        <f t="shared" si="7"/>
         <v>254524</v>
       </c>
-      <c r="U8" s="60"/>
+      <c r="U8" s="49"/>
       <c r="V8" s="25"/>
       <c r="W8" s="25"/>
       <c r="X8" s="25"/>
@@ -1929,39 +1913,39 @@
         <v>0.31</v>
       </c>
       <c r="H9" s="16">
-        <f>G9*R9</f>
+        <f t="shared" si="0"/>
         <v>78040.639999999999</v>
       </c>
       <c r="I9" s="16">
-        <f>(H9/(1-$L9))-H9</f>
+        <f t="shared" si="1"/>
         <v>11897.179999999993</v>
       </c>
       <c r="J9" s="16">
-        <f>F9*R9</f>
+        <f t="shared" si="2"/>
         <v>173703.36</v>
       </c>
       <c r="K9" s="16">
-        <f>(J9/(1-$L9))-J9</f>
+        <f t="shared" si="3"/>
         <v>26480.819999999978</v>
       </c>
       <c r="L9" s="18">
-        <f>S9/(R9+S9)</f>
+        <f t="shared" si="4"/>
         <v>0.13228228124719946</v>
       </c>
       <c r="M9" s="17">
-        <f>(O9/O8)-1</f>
+        <f t="shared" si="5"/>
         <v>0.11525538931444945</v>
       </c>
       <c r="N9" s="17">
-        <f>(P9/P8)-1</f>
+        <f t="shared" si="6"/>
         <v>7.6463897512208057E-2</v>
       </c>
       <c r="O9" s="16">
-        <f>H9/B9</f>
+        <f t="shared" si="8"/>
         <v>281227.53153153148</v>
       </c>
       <c r="P9" s="16">
-        <f>J9/D9</f>
+        <f t="shared" si="9"/>
         <v>2672359.3846153845</v>
       </c>
       <c r="Q9" s="15"/>
@@ -1972,10 +1956,10 @@
         <v>38378</v>
       </c>
       <c r="T9" s="14">
-        <f>R9+S9</f>
+        <f t="shared" si="7"/>
         <v>290122</v>
       </c>
-      <c r="U9" s="60"/>
+      <c r="U9" s="49"/>
       <c r="V9" s="25"/>
       <c r="W9" s="25"/>
       <c r="X9" s="25"/>
@@ -2000,39 +1984,39 @@
         <v>0.31</v>
       </c>
       <c r="H10" s="16">
-        <f>G10*R10</f>
+        <f t="shared" si="0"/>
         <v>85390.43</v>
       </c>
       <c r="I10" s="16">
-        <f>(H10/(1-$L10))-H10</f>
+        <f t="shared" si="1"/>
         <v>11935.929999999993</v>
       </c>
       <c r="J10" s="16">
-        <f>F10*R10</f>
+        <f t="shared" si="2"/>
         <v>190062.56999999998</v>
       </c>
       <c r="K10" s="16">
-        <f>(J10/(1-$L10))-J10</f>
+        <f t="shared" si="3"/>
         <v>26567.069999999978</v>
       </c>
       <c r="L10" s="18">
-        <f>S10/(R10+S10)</f>
+        <f t="shared" si="4"/>
         <v>0.12263820407955255</v>
       </c>
       <c r="M10" s="17">
-        <f>(O10/O9)-1</f>
+        <f t="shared" si="5"/>
         <v>0.1457912245683548</v>
       </c>
       <c r="N10" s="17">
-        <f>(P10/P9)-1</f>
+        <f t="shared" si="6"/>
         <v>9.4179007245455582E-2</v>
       </c>
       <c r="O10" s="16">
-        <f>H10/B10</f>
+        <f t="shared" si="8"/>
         <v>322228.03773584904</v>
       </c>
       <c r="P10" s="16">
-        <f>J10/D10</f>
+        <f t="shared" si="9"/>
         <v>2924039.538461538</v>
       </c>
       <c r="Q10" s="15"/>
@@ -2043,10 +2027,10 @@
         <v>38503</v>
       </c>
       <c r="T10" s="14">
-        <f>R10+S10</f>
+        <f t="shared" si="7"/>
         <v>313956</v>
       </c>
-      <c r="U10" s="60"/>
+      <c r="U10" s="49"/>
       <c r="V10" s="25"/>
       <c r="W10" s="25"/>
       <c r="X10" s="25"/>
@@ -2071,39 +2055,39 @@
         <v>0.31</v>
       </c>
       <c r="H11" s="16">
-        <f>G11*R11</f>
+        <f t="shared" si="0"/>
         <v>84867.46</v>
       </c>
       <c r="I11" s="16">
-        <f>(H11/(1-$L11))-H11</f>
+        <f t="shared" si="1"/>
         <v>6830.5399999999936</v>
       </c>
       <c r="J11" s="16">
-        <f>F11*R11</f>
+        <f t="shared" si="2"/>
         <v>188898.53999999998</v>
       </c>
       <c r="K11" s="16">
-        <f>(J11/(1-$L11))-J11</f>
+        <f t="shared" si="3"/>
         <v>15203.459999999992</v>
       </c>
       <c r="L11" s="18">
-        <f>S11/(R11+S11)</f>
+        <f t="shared" si="4"/>
         <v>7.4489519945909397E-2</v>
       </c>
       <c r="M11" s="17">
-        <f>(O11/O10)-1</f>
+        <f t="shared" si="5"/>
         <v>4.3077302760281322E-2</v>
       </c>
       <c r="N11" s="17">
-        <f>(P11/P10)-1</f>
+        <f t="shared" si="6"/>
         <v>-6.1244568038830716E-3</v>
       </c>
       <c r="O11" s="16">
-        <f>H11/B11</f>
+        <f t="shared" si="8"/>
         <v>336108.75247524754</v>
       </c>
       <c r="P11" s="16">
-        <f>J11/D11</f>
+        <f t="shared" si="9"/>
         <v>2906131.384615384</v>
       </c>
       <c r="Q11" s="15"/>
@@ -2114,10 +2098,10 @@
         <v>22034</v>
       </c>
       <c r="T11" s="14">
-        <f>R11+S11</f>
+        <f t="shared" si="7"/>
         <v>295800</v>
       </c>
-      <c r="U11" s="60"/>
+      <c r="U11" s="49"/>
       <c r="V11" s="25"/>
       <c r="W11" s="25"/>
       <c r="X11" s="25"/>
@@ -2142,39 +2126,39 @@
         <v>0.31</v>
       </c>
       <c r="H12" s="16">
-        <f>G12*R12</f>
+        <f t="shared" si="0"/>
         <v>74004.44</v>
       </c>
       <c r="I12" s="16">
-        <f>(H12/(1-$L12))-H12</f>
+        <f t="shared" si="1"/>
         <v>14682.840000000011</v>
       </c>
       <c r="J12" s="16">
-        <f>F12*R12</f>
+        <f t="shared" si="2"/>
         <v>164719.56</v>
       </c>
       <c r="K12" s="16">
-        <f>(J12/(1-$L12))-J12</f>
+        <f t="shared" si="3"/>
         <v>32681.160000000003</v>
       </c>
       <c r="L12" s="18">
-        <f>S12/(R12+S12)</f>
+        <f t="shared" si="4"/>
         <v>0.16555745085428261</v>
       </c>
       <c r="M12" s="17">
-        <f>(O12/O11)-1</f>
+        <f t="shared" si="5"/>
         <v>-8.2583148869228906E-2</v>
       </c>
       <c r="N12" s="17">
-        <f>(P12/P11)-1</f>
+        <f t="shared" si="6"/>
         <v>-0.12799982466778181</v>
       </c>
       <c r="O12" s="16">
-        <f>H12/B12</f>
+        <f t="shared" si="8"/>
         <v>308351.83333333337</v>
       </c>
       <c r="P12" s="16">
-        <f>J12/D12</f>
+        <f t="shared" si="9"/>
         <v>2534147.076923077</v>
       </c>
       <c r="Q12" s="15"/>
@@ -2185,10 +2169,10 @@
         <v>47364</v>
       </c>
       <c r="T12" s="14">
-        <f>R12+S12</f>
+        <f t="shared" si="7"/>
         <v>286088</v>
       </c>
-      <c r="U12" s="60"/>
+      <c r="U12" s="49"/>
       <c r="V12" s="25"/>
       <c r="W12" s="25"/>
       <c r="X12" s="25"/>
@@ -2213,39 +2197,39 @@
         <v>0.31</v>
       </c>
       <c r="H13" s="16">
-        <f>G13*R13</f>
+        <f t="shared" si="0"/>
         <v>83681.710000000006</v>
       </c>
       <c r="I13" s="16">
-        <f>(H13/(1-$L13))-H13</f>
+        <f t="shared" si="1"/>
         <v>12164.089999999997</v>
       </c>
       <c r="J13" s="16">
-        <f>F13*R13</f>
+        <f t="shared" si="2"/>
         <v>186259.28999999998</v>
       </c>
       <c r="K13" s="16">
-        <f>(J13/(1-$L13))-J13</f>
+        <f t="shared" si="3"/>
         <v>27074.910000000003</v>
       </c>
       <c r="L13" s="18">
-        <f>S13/(R13+S13)</f>
+        <f t="shared" si="4"/>
         <v>0.12691312504042954</v>
       </c>
       <c r="M13" s="17">
-        <f>(O13/O12)-1</f>
+        <f t="shared" si="5"/>
         <v>0.17992981525691287</v>
       </c>
       <c r="N13" s="17">
-        <f>(P13/P12)-1</f>
+        <f t="shared" si="6"/>
         <v>0.13076607295454146</v>
       </c>
       <c r="O13" s="16">
-        <f>H13/B13</f>
+        <f t="shared" si="8"/>
         <v>363833.52173913043</v>
       </c>
       <c r="P13" s="16">
-        <f>J13/D13</f>
+        <f t="shared" si="9"/>
         <v>2865527.538461538</v>
       </c>
       <c r="Q13" s="15"/>
@@ -2256,10 +2240,10 @@
         <v>39239</v>
       </c>
       <c r="T13" s="14">
-        <f>R13+S13</f>
+        <f t="shared" si="7"/>
         <v>309180</v>
       </c>
-      <c r="U13" s="60"/>
+      <c r="U13" s="49"/>
       <c r="V13" s="25"/>
       <c r="W13" s="25"/>
       <c r="X13" s="25"/>
@@ -2284,39 +2268,39 @@
         <v>0.31</v>
       </c>
       <c r="H14" s="16">
-        <f>G14*R14</f>
+        <f t="shared" si="0"/>
         <v>101260.88</v>
       </c>
       <c r="I14" s="16">
-        <f>(H14/(1-$L14))-H14</f>
+        <f t="shared" si="1"/>
         <v>16370.479999999996</v>
       </c>
       <c r="J14" s="16">
-        <f>F14*R14</f>
+        <f t="shared" si="2"/>
         <v>225387.12</v>
       </c>
       <c r="K14" s="16">
-        <f>(J14/(1-$L14))-J14</f>
+        <f t="shared" si="3"/>
         <v>36437.51999999999</v>
       </c>
       <c r="L14" s="18">
-        <f>S14/(R14+S14)</f>
+        <f t="shared" si="4"/>
         <v>0.13916765053128691</v>
       </c>
       <c r="M14" s="17">
-        <f>(O14/O13)-1</f>
+        <f t="shared" si="5"/>
         <v>0.32531676675026522</v>
       </c>
       <c r="N14" s="17">
-        <f>(P14/P13)-1</f>
+        <f t="shared" si="6"/>
         <v>0.21007183051111178</v>
       </c>
       <c r="O14" s="16">
-        <f>H14/B14</f>
+        <f t="shared" si="8"/>
         <v>482194.66666666669</v>
       </c>
       <c r="P14" s="16">
-        <f>J14/D14</f>
+        <f t="shared" si="9"/>
         <v>3467494.1538461535</v>
       </c>
       <c r="Q14" s="15"/>
@@ -2327,10 +2311,10 @@
         <v>52808</v>
       </c>
       <c r="T14" s="14">
-        <f>R14+S14</f>
+        <f t="shared" si="7"/>
         <v>379456</v>
       </c>
-      <c r="U14" s="60"/>
+      <c r="U14" s="49"/>
       <c r="V14" s="25"/>
       <c r="W14" s="25"/>
       <c r="X14" s="25"/>
@@ -2355,39 +2339,39 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="H15" s="16">
-        <f>G15*R15</f>
+        <f t="shared" si="0"/>
         <v>113234.26999999999</v>
       </c>
       <c r="I15" s="16">
-        <f>(H15/(1-$L15))-H15</f>
+        <f t="shared" si="1"/>
         <v>7261.8899999999994</v>
       </c>
       <c r="J15" s="16">
-        <f>F15*R15</f>
+        <f t="shared" si="2"/>
         <v>277228.73</v>
       </c>
       <c r="K15" s="16">
-        <f>(J15/(1-$L15))-J15</f>
+        <f t="shared" si="3"/>
         <v>17779.109999999986</v>
       </c>
       <c r="L15" s="18">
-        <f>S15/(R15+S15)</f>
+        <f t="shared" si="4"/>
         <v>6.0266567830875271E-2</v>
       </c>
       <c r="M15" s="17">
-        <f>(O15/O14)-1</f>
+        <f t="shared" si="5"/>
         <v>0.23595278692131894</v>
       </c>
       <c r="N15" s="17">
-        <f>(P15/P14)-1</f>
+        <f t="shared" si="6"/>
         <v>0.23001141325200836</v>
       </c>
       <c r="O15" s="16">
-        <f>H15/B15</f>
+        <f t="shared" si="8"/>
         <v>595969.84210526315</v>
       </c>
       <c r="P15" s="16">
-        <f>J15/D15</f>
+        <f t="shared" si="9"/>
         <v>4265057.384615384</v>
       </c>
       <c r="Q15" s="15"/>
@@ -2398,10 +2382,10 @@
         <v>25041</v>
       </c>
       <c r="T15" s="14">
-        <f>R15+S15</f>
+        <f t="shared" si="7"/>
         <v>415504</v>
       </c>
-      <c r="U15" s="60"/>
+      <c r="U15" s="49"/>
       <c r="V15" s="25"/>
       <c r="W15" s="25"/>
       <c r="X15" s="25"/>
@@ -2426,39 +2410,39 @@
         <v>0.25</v>
       </c>
       <c r="H16" s="16">
-        <f>G16*R16</f>
+        <f t="shared" si="0"/>
         <v>100477.75</v>
       </c>
       <c r="I16" s="16">
-        <f>(H16/(1-$L16))-H16</f>
+        <f t="shared" si="1"/>
         <v>8611.75</v>
       </c>
       <c r="J16" s="16">
-        <f>F16*R16</f>
+        <f t="shared" si="2"/>
         <v>301433.25</v>
       </c>
       <c r="K16" s="16">
-        <f>(J16/(1-$L16))-J16</f>
+        <f t="shared" si="3"/>
         <v>25835.25</v>
       </c>
       <c r="L16" s="18">
-        <f>S16/(R16+S16)</f>
+        <f t="shared" si="4"/>
         <v>7.8942061334958916E-2</v>
       </c>
       <c r="M16" s="17">
-        <f>(O16/O15)-1</f>
+        <f t="shared" si="5"/>
         <v>1.258474394981568E-2</v>
       </c>
       <c r="N16" s="17">
-        <f>(P16/P15)-1</f>
+        <f t="shared" si="6"/>
         <v>8.7308844216831494E-2</v>
       </c>
       <c r="O16" s="16">
-        <f>H16/B16</f>
+        <f t="shared" si="8"/>
         <v>603469.96996996994</v>
       </c>
       <c r="P16" s="16">
-        <f>J16/D16</f>
+        <f t="shared" si="9"/>
         <v>4637434.615384615</v>
       </c>
       <c r="Q16" s="15"/>
@@ -2469,10 +2453,10 @@
         <v>34447</v>
       </c>
       <c r="T16" s="14">
-        <f>R16+S16</f>
+        <f t="shared" si="7"/>
         <v>436358</v>
       </c>
-      <c r="U16" s="60"/>
+      <c r="U16" s="49"/>
       <c r="V16" s="25"/>
       <c r="W16" s="25"/>
       <c r="X16" s="25"/>
@@ -2497,39 +2481,39 @@
         <v>0.25</v>
       </c>
       <c r="H17" s="16">
-        <f>G17*R17</f>
+        <f t="shared" si="0"/>
         <v>94033.25</v>
       </c>
       <c r="I17" s="16">
-        <f>(H17/(1-$L17))-H17</f>
+        <f t="shared" si="1"/>
         <v>5673.5</v>
       </c>
       <c r="J17" s="16">
-        <f>F17*R17</f>
+        <f t="shared" si="2"/>
         <v>282099.75</v>
       </c>
       <c r="K17" s="16">
-        <f>(J17/(1-$L17))-J17</f>
+        <f t="shared" si="3"/>
         <v>17020.5</v>
       </c>
       <c r="L17" s="18">
-        <f>S17/(R17+S17)</f>
+        <f t="shared" si="4"/>
         <v>5.6901864718286378E-2</v>
       </c>
       <c r="M17" s="17">
-        <f>(O17/O16)-1</f>
+        <f t="shared" si="5"/>
         <v>1.1824199820422931E-2</v>
       </c>
       <c r="N17" s="17">
-        <f>(P17/P16)-1</f>
+        <f t="shared" si="6"/>
         <v>-6.413857794387301E-2</v>
       </c>
       <c r="O17" s="16">
-        <f>H17/B17</f>
+        <f t="shared" si="8"/>
         <v>610605.51948051946</v>
       </c>
       <c r="P17" s="16">
-        <f>J17/D17</f>
+        <f t="shared" si="9"/>
         <v>4339996.153846154</v>
       </c>
       <c r="Q17" s="15"/>
@@ -2540,10 +2524,10 @@
         <v>22694</v>
       </c>
       <c r="T17" s="14">
-        <f>R17+S17</f>
+        <f t="shared" si="7"/>
         <v>398827</v>
       </c>
-      <c r="U17" s="60"/>
+      <c r="U17" s="49"/>
       <c r="V17" s="25"/>
       <c r="W17" s="25"/>
       <c r="X17" s="25"/>
@@ -2568,39 +2552,39 @@
         <v>0.25</v>
       </c>
       <c r="H18" s="16">
-        <f>G18*R18</f>
+        <f t="shared" si="0"/>
         <v>91768.5</v>
       </c>
       <c r="I18" s="16">
-        <f>(H18/(1-$L18))-H18</f>
+        <f t="shared" si="1"/>
         <v>4729</v>
       </c>
       <c r="J18" s="16">
-        <f>F18*R18</f>
+        <f t="shared" si="2"/>
         <v>275305.5</v>
       </c>
       <c r="K18" s="16">
-        <f>(J18/(1-$L18))-J18</f>
+        <f t="shared" si="3"/>
         <v>14187</v>
       </c>
       <c r="L18" s="18">
-        <f>S18/(R18+S18)</f>
+        <f t="shared" si="4"/>
         <v>4.9006450944324979E-2</v>
       </c>
       <c r="M18" s="17">
-        <f>(O18/O17)-1</f>
+        <f t="shared" si="5"/>
         <v>6.2127044960480049E-2</v>
       </c>
       <c r="N18" s="17">
-        <f>(P18/P17)-1</f>
+        <f t="shared" si="6"/>
         <v>-1.6519329907982327E-2</v>
       </c>
       <c r="O18" s="16">
-        <f>H18/B18</f>
+        <f t="shared" si="8"/>
         <v>648540.63604240294</v>
       </c>
       <c r="P18" s="16">
-        <f>J18/D18</f>
+        <f t="shared" si="9"/>
         <v>4268302.3255813951</v>
       </c>
       <c r="Q18" s="15"/>
@@ -2611,10 +2595,10 @@
         <v>18916</v>
       </c>
       <c r="T18" s="14">
-        <f>R18+S18</f>
+        <f t="shared" si="7"/>
         <v>385990</v>
       </c>
-      <c r="U18" s="60"/>
+      <c r="U18" s="49"/>
       <c r="V18" s="25"/>
       <c r="W18" s="25"/>
       <c r="X18" s="25"/>
@@ -2639,39 +2623,39 @@
         <v>0.26</v>
       </c>
       <c r="H19" s="16">
-        <f>G19*R19</f>
+        <f t="shared" si="0"/>
         <v>85611.5</v>
       </c>
       <c r="I19" s="16">
-        <f>(H19/(1-$L19))-H19</f>
+        <f t="shared" si="1"/>
         <v>9211.2799999999988</v>
       </c>
       <c r="J19" s="16">
-        <f>F19*R19</f>
+        <f t="shared" si="2"/>
         <v>243663.5</v>
       </c>
       <c r="K19" s="16">
-        <f>(J19/(1-$L19))-J19</f>
+        <f t="shared" si="3"/>
         <v>26216.719999999972</v>
       </c>
       <c r="L19" s="18">
-        <f>S19/(R19+S19)</f>
+        <f t="shared" si="4"/>
         <v>9.7142058058200781E-2</v>
       </c>
       <c r="M19" s="17">
-        <f>(O19/O18)-1</f>
+        <f t="shared" si="5"/>
         <v>-6.7092738793812723E-2</v>
       </c>
       <c r="N19" s="17">
-        <f>(P19/P18)-1</f>
+        <f t="shared" si="6"/>
         <v>-0.11493413680438636</v>
       </c>
       <c r="O19" s="16">
-        <f>H19/B19</f>
+        <f t="shared" si="8"/>
         <v>605028.26855123683</v>
       </c>
       <c r="P19" s="16">
-        <f>J19/D19</f>
+        <f t="shared" si="9"/>
         <v>3777728.6821705424</v>
       </c>
       <c r="Q19" s="15"/>
@@ -2682,12 +2666,12 @@
         <v>35428</v>
       </c>
       <c r="T19" s="14">
-        <f>R19+S19</f>
+        <f t="shared" si="7"/>
         <v>364703</v>
       </c>
-      <c r="U19" s="60"/>
-      <c r="V19" s="44"/>
-      <c r="W19" s="45"/>
+      <c r="U19" s="49"/>
+      <c r="V19" s="43"/>
+      <c r="W19" s="44"/>
       <c r="X19" s="25"/>
       <c r="Y19" s="42"/>
     </row>
@@ -2710,39 +2694,39 @@
         <v>0.26</v>
       </c>
       <c r="H20" s="16">
-        <f>G20*R20</f>
+        <f t="shared" si="0"/>
         <v>87098.96</v>
       </c>
       <c r="I20" s="16">
-        <f>(H20/(1-$L20))-H20</f>
+        <f t="shared" si="1"/>
         <v>10907</v>
       </c>
       <c r="J20" s="16">
-        <f>F20*R20</f>
+        <f t="shared" si="2"/>
         <v>247897.04</v>
       </c>
       <c r="K20" s="16">
-        <f>(J20/(1-$L20))-J20</f>
+        <f t="shared" si="3"/>
         <v>31043.000000000029</v>
       </c>
       <c r="L20" s="18">
-        <f>S20/(R20+S20)</f>
+        <f t="shared" si="4"/>
         <v>0.11128915017005088</v>
       </c>
       <c r="M20" s="17">
-        <f>(O20/O19)-1</f>
+        <f t="shared" si="5"/>
         <v>1.7374534963176869E-2</v>
       </c>
       <c r="N20" s="17">
-        <f>(P20/P19)-1</f>
+        <f t="shared" si="6"/>
         <v>1.7374534963176869E-2</v>
       </c>
       <c r="O20" s="16">
-        <f>H20/B20</f>
+        <f t="shared" si="8"/>
         <v>615540.35335689061</v>
       </c>
       <c r="P20" s="16">
-        <f>J20/D20</f>
+        <f t="shared" si="9"/>
         <v>3843364.9612403102</v>
       </c>
       <c r="Q20" s="15"/>
@@ -2753,10 +2737,10 @@
         <v>41950</v>
       </c>
       <c r="T20" s="14">
-        <f>R20+S20</f>
+        <f t="shared" si="7"/>
         <v>376946</v>
       </c>
-      <c r="U20" s="60"/>
+      <c r="U20" s="49"/>
       <c r="V20" s="42"/>
       <c r="W20" s="42"/>
       <c r="X20" s="25"/>
@@ -2781,39 +2765,39 @@
         <v>0.26</v>
       </c>
       <c r="H21" s="16">
-        <f>G21*R21</f>
+        <f t="shared" si="0"/>
         <v>96249.14</v>
       </c>
       <c r="I21" s="16">
-        <f>(H21/(1-$L21))-H21</f>
+        <f t="shared" si="1"/>
         <v>4991.2200000000012</v>
       </c>
       <c r="J21" s="16">
-        <f>F21*R21</f>
+        <f t="shared" si="2"/>
         <v>273939.86</v>
       </c>
       <c r="K21" s="16">
-        <f>(J21/(1-$L21))-J21</f>
+        <f t="shared" si="3"/>
         <v>14205.780000000028</v>
       </c>
       <c r="L21" s="18">
-        <f>S21/(R21+S21)</f>
+        <f t="shared" si="4"/>
         <v>4.9300693912980947E-2</v>
       </c>
       <c r="M21" s="17">
-        <f>(O21/O20)-1</f>
+        <f t="shared" si="5"/>
         <v>0.10505498573117289</v>
       </c>
       <c r="N21" s="17">
-        <f>(P21/P20)-1</f>
+        <f t="shared" si="6"/>
         <v>0.10505498573117267</v>
       </c>
       <c r="O21" s="16">
-        <f>H21/B21</f>
+        <f t="shared" si="8"/>
         <v>680205.93639575981</v>
       </c>
       <c r="P21" s="16">
-        <f>J21/D21</f>
+        <f t="shared" si="9"/>
         <v>4247129.6124031004</v>
       </c>
       <c r="Q21" s="15"/>
@@ -2824,12 +2808,12 @@
         <v>19197</v>
       </c>
       <c r="T21" s="14">
-        <f>R21+S21</f>
+        <f t="shared" si="7"/>
         <v>389386</v>
       </c>
-      <c r="U21" s="60"/>
+      <c r="U21" s="49"/>
       <c r="V21" s="24"/>
-      <c r="W21" s="44"/>
+      <c r="W21" s="43"/>
       <c r="X21" s="25"/>
       <c r="Y21" s="42"/>
     </row>
@@ -2852,39 +2836,39 @@
         <v>0.26</v>
       </c>
       <c r="H22" s="16">
-        <f>G22*R22</f>
+        <f t="shared" si="0"/>
         <v>107050.06</v>
       </c>
       <c r="I22" s="16">
-        <f>(H22/(1-$L22))-H22</f>
+        <f t="shared" si="1"/>
         <v>10186.800000000003</v>
       </c>
       <c r="J22" s="16">
-        <f>F22*R22</f>
+        <f t="shared" si="2"/>
         <v>304680.94</v>
       </c>
       <c r="K22" s="16">
-        <f>(J22/(1-$L22))-J22</f>
+        <f t="shared" si="3"/>
         <v>28993.200000000012</v>
       </c>
       <c r="L22" s="18">
-        <f>S22/(R22+S22)</f>
+        <f t="shared" si="4"/>
         <v>8.6890761147987078E-2</v>
       </c>
       <c r="M22" s="17">
-        <f>(O22/O21)-1</f>
+        <f t="shared" si="5"/>
         <v>0.11221835332762442</v>
       </c>
       <c r="N22" s="17">
-        <f>(P22/P21)-1</f>
+        <f t="shared" si="6"/>
         <v>0.11221835332762464</v>
       </c>
       <c r="O22" s="16">
-        <f>H22/B22</f>
+        <f t="shared" si="8"/>
         <v>756537.52650176687</v>
       </c>
       <c r="P22" s="16">
-        <f>J22/D22</f>
+        <f t="shared" si="9"/>
         <v>4723735.503875969</v>
       </c>
       <c r="Q22" s="15"/>
@@ -2895,10 +2879,10 @@
         <v>39180</v>
       </c>
       <c r="T22" s="14">
-        <f>R22+S22</f>
+        <f t="shared" si="7"/>
         <v>450911</v>
       </c>
-      <c r="U22" s="60"/>
+      <c r="U22" s="49"/>
       <c r="V22" s="42"/>
       <c r="W22" s="42"/>
       <c r="X22" s="25"/>
@@ -2923,39 +2907,39 @@
         <v>0.26</v>
       </c>
       <c r="H23" s="16">
-        <f>G23*R23</f>
+        <f t="shared" si="0"/>
         <v>109477.16</v>
       </c>
       <c r="I23" s="16">
-        <f>(H23/(1-$L23))-H23</f>
+        <f t="shared" si="1"/>
         <v>10553.140000000014</v>
       </c>
       <c r="J23" s="16">
-        <f>F23*R23</f>
+        <f t="shared" si="2"/>
         <v>311588.83999999997</v>
       </c>
       <c r="K23" s="16">
-        <f>(J23/(1-$L23))-J23</f>
+        <f t="shared" si="3"/>
         <v>30035.860000000044</v>
       </c>
       <c r="L23" s="18">
-        <f>S23/(R23+S23)</f>
+        <f t="shared" si="4"/>
         <v>8.7920633373406554E-2</v>
       </c>
       <c r="M23" s="17">
-        <f>(O23/O22)-1</f>
+        <f t="shared" si="5"/>
         <v>2.2672570197531883E-2</v>
       </c>
       <c r="N23" s="17">
-        <f>(P23/P22)-1</f>
+        <f t="shared" si="6"/>
         <v>2.5853511317897482E-2</v>
       </c>
       <c r="O23" s="16">
-        <f>H23/B23</f>
+        <f t="shared" si="8"/>
         <v>773690.17667844531</v>
       </c>
       <c r="P23" s="16">
-        <f>J23/D23</f>
+        <f t="shared" si="9"/>
         <v>4845860.6531881802</v>
       </c>
       <c r="Q23" s="15"/>
@@ -2966,12 +2950,12 @@
         <v>40589</v>
       </c>
       <c r="T23" s="14">
-        <f>R23+S23</f>
+        <f t="shared" si="7"/>
         <v>461655</v>
       </c>
-      <c r="U23" s="60"/>
+      <c r="U23" s="49"/>
       <c r="V23" s="24"/>
-      <c r="W23" s="44"/>
+      <c r="W23" s="43"/>
       <c r="X23" s="42"/>
       <c r="Y23" s="42"/>
     </row>
@@ -2994,39 +2978,39 @@
         <v>0.26</v>
       </c>
       <c r="H24" s="16">
-        <f>G24*R24</f>
+        <f t="shared" si="0"/>
         <v>104551.46</v>
       </c>
       <c r="I24" s="16">
-        <f>(H24/(1-$L24))-H24</f>
+        <f t="shared" si="1"/>
         <v>9389.64</v>
       </c>
       <c r="J24" s="16">
-        <f>F24*R24</f>
+        <f t="shared" si="2"/>
         <v>297569.53999999998</v>
       </c>
       <c r="K24" s="16">
-        <f>(J24/(1-$L24))-J24</f>
+        <f t="shared" si="3"/>
         <v>26724.359999999986</v>
       </c>
       <c r="L24" s="18">
-        <f>S24/(R24+S24)</f>
+        <f t="shared" si="4"/>
         <v>8.2407840542174857E-2</v>
       </c>
       <c r="M24" s="17">
-        <f>(O24/O23)-1</f>
+        <f t="shared" si="5"/>
         <v>-4.4992946473949358E-2</v>
       </c>
       <c r="N24" s="17">
-        <f>(P24/P23)-1</f>
+        <f t="shared" si="6"/>
         <v>-4.2013205277300347E-2</v>
       </c>
       <c r="O24" s="16">
-        <f>H24/B24</f>
+        <f t="shared" si="8"/>
         <v>738879.57597173157</v>
       </c>
       <c r="P24" s="16">
-        <f>J24/D24</f>
+        <f t="shared" si="9"/>
         <v>4642270.5148205925</v>
       </c>
       <c r="Q24" s="15"/>
@@ -3037,10 +3021,10 @@
         <v>36114</v>
       </c>
       <c r="T24" s="14">
-        <f>R24+S24</f>
+        <f t="shared" si="7"/>
         <v>438235</v>
       </c>
-      <c r="U24" s="60"/>
+      <c r="U24" s="49"/>
       <c r="V24" s="42"/>
       <c r="W24" s="42"/>
       <c r="X24" s="42"/>
@@ -3065,39 +3049,39 @@
         <v>0.26</v>
       </c>
       <c r="H25" s="16">
-        <f>G25*R25</f>
+        <f t="shared" si="0"/>
         <v>111054.84000000001</v>
       </c>
       <c r="I25" s="16">
-        <f>(H25/(1-$L25))-H25</f>
+        <f t="shared" si="1"/>
         <v>12229.62000000001</v>
       </c>
       <c r="J25" s="16">
-        <f>F25*R25</f>
+        <f t="shared" si="2"/>
         <v>316079.15999999997</v>
       </c>
       <c r="K25" s="16">
-        <f>(J25/(1-$L25))-J25</f>
+        <f t="shared" si="3"/>
         <v>34807.380000000005</v>
       </c>
       <c r="L25" s="18">
-        <f>S25/(R25+S25)</f>
+        <f t="shared" si="4"/>
         <v>9.919839045407669E-2</v>
       </c>
       <c r="M25" s="17">
-        <f>(O25/O24)-1</f>
+        <f t="shared" si="5"/>
         <v>6.2202670340519406E-2</v>
       </c>
       <c r="N25" s="17">
-        <f>(P25/P24)-1</f>
+        <f t="shared" si="6"/>
         <v>6.5527248338455246E-2</v>
       </c>
       <c r="O25" s="16">
-        <f>H25/B25</f>
+        <f t="shared" si="8"/>
         <v>784839.85865724401</v>
       </c>
       <c r="P25" s="16">
-        <f>J25/D25</f>
+        <f t="shared" si="9"/>
         <v>4946465.7276995303</v>
       </c>
       <c r="Q25" s="15"/>
@@ -3108,12 +3092,12 @@
         <v>47037</v>
       </c>
       <c r="T25" s="14">
-        <f>R25+S25</f>
+        <f t="shared" si="7"/>
         <v>474171</v>
       </c>
-      <c r="U25" s="60"/>
+      <c r="U25" s="49"/>
       <c r="V25" s="24"/>
-      <c r="W25" s="44"/>
+      <c r="W25" s="43"/>
       <c r="X25" s="42"/>
       <c r="Y25" s="42"/>
     </row>
@@ -3136,39 +3120,39 @@
         <v>0.27</v>
       </c>
       <c r="H26" s="16">
-        <f>G26*R26</f>
+        <f t="shared" si="0"/>
         <v>107091.45000000001</v>
       </c>
       <c r="I26" s="16">
-        <f>(H26/(1-$L26))-H26</f>
+        <f t="shared" si="1"/>
         <v>5640.5699999999924</v>
       </c>
       <c r="J26" s="16">
-        <f>F26*R26</f>
+        <f t="shared" si="2"/>
         <v>289543.55</v>
       </c>
       <c r="K26" s="16">
-        <f>(J26/(1-$L26))-J26</f>
+        <f t="shared" si="3"/>
         <v>15250.429999999993</v>
       </c>
       <c r="L26" s="18">
-        <f>S26/(R26+S26)</f>
+        <f t="shared" si="4"/>
         <v>5.0035207388282404E-2</v>
       </c>
       <c r="M26" s="17">
-        <f>(O26/O25)-1</f>
+        <f t="shared" si="5"/>
         <v>-3.5688584126545075E-2</v>
       </c>
       <c r="N26" s="17">
-        <f>(P26/P25)-1</f>
+        <f t="shared" si="6"/>
         <v>-7.8182040290309618E-2</v>
       </c>
       <c r="O26" s="16">
-        <f>H26/B26</f>
+        <f t="shared" si="8"/>
         <v>756830.0353356892</v>
       </c>
       <c r="P26" s="16">
-        <f>J26/D26</f>
+        <f t="shared" si="9"/>
         <v>4559740.94488189</v>
       </c>
       <c r="Q26" s="15"/>
@@ -3179,12 +3163,12 @@
         <v>20891</v>
       </c>
       <c r="T26" s="14">
-        <f>R26+S26</f>
+        <f t="shared" si="7"/>
         <v>417526</v>
       </c>
-      <c r="U26" s="60"/>
+      <c r="U26" s="49"/>
       <c r="V26" s="24"/>
-      <c r="W26" s="44"/>
+      <c r="W26" s="43"/>
       <c r="X26" s="42"/>
       <c r="Y26" s="42"/>
     </row>
@@ -3207,39 +3191,39 @@
         <v>0.27</v>
       </c>
       <c r="H27" s="16">
-        <f>G27*R27</f>
+        <f t="shared" si="0"/>
         <v>115792.47</v>
       </c>
       <c r="I27" s="16">
-        <f>(H27/(1-$L27))-H27</f>
+        <f t="shared" si="1"/>
         <v>4646.6999999999971</v>
       </c>
       <c r="J27" s="16">
-        <f>F27*R27</f>
+        <f t="shared" si="2"/>
         <v>313068.52999999997</v>
       </c>
       <c r="K27" s="16">
-        <f>(J27/(1-$L27))-J27</f>
+        <f t="shared" si="3"/>
         <v>12563.299999999988</v>
       </c>
       <c r="L27" s="18">
-        <f>S27/(R27+S27)</f>
+        <f t="shared" si="4"/>
         <v>3.8581302079713768E-2</v>
       </c>
       <c r="M27" s="17">
-        <f>(O27/O26)-1</f>
+        <f t="shared" si="5"/>
         <v>8.124850303175446E-2</v>
       </c>
       <c r="N27" s="17">
-        <f>(P27/P26)-1</f>
+        <f t="shared" si="6"/>
         <v>8.9829840357403379E-2</v>
       </c>
       <c r="O27" s="16">
-        <f>H27/B27</f>
+        <f t="shared" si="8"/>
         <v>818321.34275618382</v>
       </c>
       <c r="P27" s="16">
-        <f>J27/D27</f>
+        <f t="shared" si="9"/>
         <v>4969341.7460317453</v>
       </c>
       <c r="Q27" s="15"/>
@@ -3250,12 +3234,12 @@
         <v>17210</v>
       </c>
       <c r="T27" s="14">
-        <f>R27+S27</f>
+        <f t="shared" si="7"/>
         <v>446071</v>
       </c>
-      <c r="U27" s="60"/>
+      <c r="U27" s="49"/>
       <c r="V27" s="24"/>
-      <c r="W27" s="44"/>
+      <c r="W27" s="43"/>
       <c r="X27" s="42"/>
       <c r="Y27" s="42"/>
     </row>
@@ -3278,39 +3262,39 @@
         <v>0.27</v>
       </c>
       <c r="H28" s="16">
-        <f>G28*R28</f>
+        <f t="shared" si="0"/>
         <v>136796.58000000002</v>
       </c>
       <c r="I28" s="16">
-        <f>(H28/(1-$L28))-H28</f>
+        <f t="shared" si="1"/>
         <v>9239.3999999999942</v>
       </c>
       <c r="J28" s="16">
-        <f>F28*R28</f>
+        <f t="shared" si="2"/>
         <v>369857.42</v>
       </c>
       <c r="K28" s="16">
-        <f>(J28/(1-$L28))-J28</f>
+        <f t="shared" si="3"/>
         <v>24980.600000000035</v>
       </c>
       <c r="L28" s="18">
-        <f>S28/(R28+S28)</f>
+        <f t="shared" si="4"/>
         <v>6.3267969989313597E-2</v>
       </c>
       <c r="M28" s="17">
-        <f>(O28/O27)-1</f>
+        <f t="shared" si="5"/>
         <v>0.1813944378248431</v>
       </c>
       <c r="N28" s="17">
-        <f>(P28/P27)-1</f>
+        <f t="shared" si="6"/>
         <v>0.19084559332744178</v>
       </c>
       <c r="O28" s="16">
-        <f>H28/B28</f>
+        <f t="shared" si="8"/>
         <v>966760.28268551256</v>
       </c>
       <c r="P28" s="16">
-        <f>J28/D28</f>
+        <f t="shared" si="9"/>
         <v>5917718.7199999997</v>
       </c>
       <c r="Q28" s="15"/>
@@ -3321,12 +3305,12 @@
         <v>34220</v>
       </c>
       <c r="T28" s="14">
-        <f>R28+S28</f>
+        <f t="shared" si="7"/>
         <v>540874</v>
       </c>
-      <c r="U28" s="60"/>
+      <c r="U28" s="49"/>
       <c r="V28" s="24"/>
-      <c r="W28" s="44"/>
+      <c r="W28" s="43"/>
       <c r="X28" s="42"/>
       <c r="Y28" s="42"/>
     </row>
@@ -3349,118 +3333,115 @@
         <v>0.27</v>
       </c>
       <c r="H29" s="16">
-        <f>G29*R29</f>
+        <f t="shared" si="0"/>
         <v>133619.76</v>
       </c>
       <c r="I29" s="16">
-        <f>(H29/(1-$L29))-H29</f>
+        <f t="shared" si="1"/>
         <v>10624.76999999999</v>
       </c>
       <c r="J29" s="16">
-        <f>F29*R29</f>
+        <f t="shared" si="2"/>
         <v>361268.24</v>
       </c>
       <c r="K29" s="16">
-        <f>(J29/(1-$L29))-J29</f>
+        <f t="shared" si="3"/>
         <v>28726.229999999981</v>
       </c>
       <c r="L29" s="18">
-        <f>S29/(R29+S29)</f>
+        <f t="shared" si="4"/>
         <v>7.365804443329671E-2</v>
       </c>
       <c r="M29" s="17">
-        <f>(O29/O28)-1</f>
+        <f t="shared" si="5"/>
         <v>-2.3222948994777615E-2</v>
       </c>
       <c r="N29" s="17">
-        <f>(P29/P28)-1</f>
+        <f t="shared" si="6"/>
         <v>-1.5345714712477254E-2</v>
       </c>
       <c r="O29" s="16">
-        <f>H29/B29</f>
+        <f t="shared" si="8"/>
         <v>944309.25795053015</v>
       </c>
       <c r="P29" s="16">
-        <f>J29/D29</f>
+        <f t="shared" si="9"/>
         <v>5826907.0967741935</v>
       </c>
       <c r="Q29" s="15"/>
-      <c r="R29" s="46">
+      <c r="R29" s="45">
         <f>225683+269205</f>
         <v>494888</v>
       </c>
-      <c r="S29" s="46">
+      <c r="S29" s="45">
         <v>39351</v>
       </c>
       <c r="T29" s="14">
-        <f>R29+S29</f>
+        <f t="shared" si="7"/>
         <v>534239</v>
       </c>
-      <c r="U29" s="61"/>
+      <c r="U29" s="49"/>
       <c r="V29" s="24"/>
-      <c r="W29" s="44"/>
+      <c r="W29" s="43"/>
       <c r="X29" s="42"/>
       <c r="Y29" s="42"/>
     </row>
     <row r="30" spans="1:25" x14ac:dyDescent="0.15">
-      <c r="A30" s="47" t="s">
+      <c r="A30" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="B30" s="48">
+      <c r="B30" s="52">
         <v>0.14149999999999999</v>
       </c>
-      <c r="C30" s="49"/>
-      <c r="D30" s="50">
+      <c r="C30" s="53"/>
+      <c r="D30" s="54">
         <v>6.2E-2</v>
       </c>
-      <c r="E30" s="50"/>
-      <c r="F30" s="51">
+      <c r="E30" s="54"/>
+      <c r="F30" s="55">
         <v>0.73</v>
       </c>
-      <c r="G30" s="51">
+      <c r="G30" s="55">
         <v>0.27</v>
       </c>
-      <c r="H30" s="52">
-        <v>129490.90941600001</v>
-      </c>
-      <c r="I30" s="53">
-        <v>10296.464606999989</v>
-      </c>
-      <c r="J30" s="53">
-        <v>350105.05138399999</v>
-      </c>
-      <c r="K30" s="53">
-        <v>27838.589492999981</v>
-      </c>
-      <c r="L30" s="54">
-        <v>7.3658044433296654E-2</v>
-      </c>
-      <c r="M30" s="55">
-        <v>-3.09E-2</v>
-      </c>
-      <c r="N30" s="55">
-        <v>-3.09E-2</v>
-      </c>
-      <c r="O30" s="53">
-        <v>915130.10187985876</v>
-      </c>
-      <c r="P30" s="53">
-        <v>5646855.6674838709</v>
-      </c>
-      <c r="Q30" s="56"/>
-      <c r="R30" s="57">
-        <v>479595.9608</v>
-      </c>
-      <c r="S30" s="57">
-        <v>38135.054099999972</v>
-      </c>
-      <c r="T30" s="58">
-        <f>R30+S30</f>
-        <v>517731.01489999995</v>
-      </c>
-      <c r="U30" s="62" t="s">
-        <v>47</v>
-      </c>
+      <c r="H30" s="56">
+        <v>131613.39000000001</v>
+      </c>
+      <c r="I30" s="57">
+        <v>14618.339999999997</v>
+      </c>
+      <c r="J30" s="57">
+        <v>355843.61</v>
+      </c>
+      <c r="K30" s="57">
+        <v>39523.659999999974</v>
+      </c>
+      <c r="L30" s="58">
+        <v>9.9966949717410852E-2</v>
+      </c>
+      <c r="M30" s="59">
+        <v>-1.501551866280848E-2</v>
+      </c>
+      <c r="N30" s="59">
+        <v>-1.5015518662808591E-2</v>
+      </c>
+      <c r="O30" s="57">
+        <v>930129.96466431115</v>
+      </c>
+      <c r="P30" s="57">
+        <v>5739413.064516129</v>
+      </c>
+      <c r="Q30" s="60"/>
+      <c r="R30" s="45">
+        <v>487457</v>
+      </c>
+      <c r="S30" s="45">
+        <v>54142</v>
+      </c>
+      <c r="T30" s="61">
+        <v>541599</v>
+      </c>
+      <c r="U30" s="46"/>
       <c r="V30" s="42"/>
       <c r="W30" s="42"/>
       <c r="X30" s="42"/>
@@ -3482,7 +3463,7 @@
       <c r="O31" s="13"/>
       <c r="P31" s="13"/>
       <c r="T31" s="3"/>
-      <c r="U31" s="42"/>
+      <c r="U31" s="50"/>
       <c r="V31" s="42"/>
       <c r="W31" s="42"/>
       <c r="X31" s="42"/>
@@ -3509,7 +3490,7 @@
       <c r="R32" s="3"/>
       <c r="S32" s="3"/>
       <c r="T32" s="3"/>
-      <c r="U32" s="44"/>
+      <c r="U32" s="42"/>
       <c r="V32" s="42"/>
       <c r="W32" s="42"/>
       <c r="X32" s="42"/>
@@ -3536,7 +3517,7 @@
       <c r="R33" s="3"/>
       <c r="S33" s="3"/>
       <c r="T33" s="3"/>
-      <c r="U33" s="44"/>
+      <c r="U33" s="43"/>
       <c r="V33" s="42"/>
       <c r="W33" s="42"/>
       <c r="X33" s="42"/>
@@ -3561,7 +3542,7 @@
       <c r="R34" s="3"/>
       <c r="S34" s="3"/>
       <c r="T34" s="3"/>
-      <c r="U34" s="44"/>
+      <c r="U34" s="43"/>
       <c r="V34" s="42"/>
       <c r="W34" s="42"/>
       <c r="X34" s="42"/>
@@ -3588,7 +3569,7 @@
       <c r="R35" s="3"/>
       <c r="S35" s="3"/>
       <c r="T35" s="3"/>
-      <c r="U35" s="44"/>
+      <c r="U35" s="43"/>
       <c r="V35" s="42"/>
       <c r="W35" s="42"/>
       <c r="X35" s="42"/>
@@ -3615,7 +3596,7 @@
       <c r="R36" s="3"/>
       <c r="S36" s="3"/>
       <c r="T36" s="3"/>
-      <c r="U36" s="44"/>
+      <c r="U36" s="43"/>
       <c r="V36" s="42"/>
       <c r="W36" s="42"/>
       <c r="X36" s="42"/>
@@ -3642,7 +3623,7 @@
       <c r="R37" s="3"/>
       <c r="S37" s="3"/>
       <c r="T37" s="3"/>
-      <c r="U37" s="44"/>
+      <c r="U37" s="43"/>
       <c r="V37" s="42"/>
       <c r="W37" s="42"/>
       <c r="X37" s="42"/>
@@ -3669,7 +3650,7 @@
       <c r="R38" s="3"/>
       <c r="S38" s="3"/>
       <c r="T38" s="3"/>
-      <c r="U38" s="44"/>
+      <c r="U38" s="43"/>
       <c r="V38" s="42"/>
       <c r="W38" s="42"/>
       <c r="X38" s="42"/>
@@ -3696,7 +3677,7 @@
       <c r="R39" s="3"/>
       <c r="S39" s="3"/>
       <c r="T39" s="3"/>
-      <c r="U39" s="44"/>
+      <c r="U39" s="43"/>
       <c r="V39" s="42"/>
       <c r="W39" s="42"/>
       <c r="X39" s="42"/>
@@ -3723,7 +3704,7 @@
       <c r="R40" s="3"/>
       <c r="S40" s="3"/>
       <c r="T40" s="3"/>
-      <c r="U40" s="44"/>
+      <c r="U40" s="43"/>
       <c r="V40" s="42"/>
       <c r="W40" s="42"/>
       <c r="X40" s="42"/>
@@ -3750,7 +3731,7 @@
       <c r="R41" s="3"/>
       <c r="S41" s="3"/>
       <c r="T41" s="3"/>
-      <c r="U41" s="44"/>
+      <c r="U41" s="43"/>
       <c r="V41" s="42"/>
       <c r="W41" s="42"/>
       <c r="X41" s="42"/>
@@ -3777,7 +3758,7 @@
       <c r="R42" s="3"/>
       <c r="S42" s="3"/>
       <c r="T42" s="3"/>
-      <c r="U42" s="44"/>
+      <c r="U42" s="43"/>
       <c r="V42" s="42"/>
       <c r="W42" s="42"/>
       <c r="X42" s="42"/>
@@ -3804,7 +3785,7 @@
       <c r="R43" s="3"/>
       <c r="S43" s="3"/>
       <c r="T43" s="3"/>
-      <c r="U43" s="44"/>
+      <c r="U43" s="43"/>
       <c r="V43" s="42"/>
       <c r="W43" s="42"/>
       <c r="X43" s="42"/>
@@ -3831,7 +3812,7 @@
       <c r="R44" s="3"/>
       <c r="S44" s="3"/>
       <c r="T44" s="3"/>
-      <c r="U44" s="44"/>
+      <c r="U44" s="43"/>
       <c r="V44" s="42"/>
       <c r="W44" s="42"/>
       <c r="X44" s="42"/>
@@ -3858,7 +3839,7 @@
       <c r="R45" s="3"/>
       <c r="S45" s="3"/>
       <c r="T45" s="3"/>
-      <c r="U45" s="44"/>
+      <c r="U45" s="43"/>
       <c r="V45" s="42"/>
       <c r="W45" s="42"/>
       <c r="X45" s="42"/>
@@ -3885,7 +3866,7 @@
       <c r="R46" s="3"/>
       <c r="S46" s="3"/>
       <c r="T46" s="3"/>
-      <c r="U46" s="44"/>
+      <c r="U46" s="43"/>
       <c r="V46" s="42"/>
       <c r="W46" s="42"/>
       <c r="X46" s="42"/>
@@ -3912,7 +3893,7 @@
       <c r="R47" s="3"/>
       <c r="S47" s="3"/>
       <c r="T47" s="3"/>
-      <c r="U47" s="3"/>
+      <c r="U47" s="43"/>
     </row>
     <row r="48" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A48" s="3"/>
@@ -5616,6 +5597,9 @@
       <c r="T121" s="3"/>
       <c r="U121" s="3"/>
     </row>
+    <row r="122" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="U122" s="3"/>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="U3:W3"/>

</xml_diff>

<commit_message>
reorg and update for FY24-FY28 plan
</commit_message>
<xml_diff>
--- a/data/01_raw/historical/BIRT-splits.xlsx
+++ b/data/01_raw/historical/BIRT-splits.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicholashand/LocalWork/Analysis/five-year-plan-analysis/data/01_raw/historical/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CF35DA1-CBB0-1E4E-942C-7F0C7271230E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B94C1599-67D0-F844-8A1C-E4948F830563}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7840" yWindow="2100" windowWidth="26840" windowHeight="15440" activeTab="1" xr2:uid="{1580F8C4-AF3E-5F4A-A010-F100369F5510}"/>
+    <workbookView xWindow="1960" yWindow="2100" windowWidth="26840" windowHeight="15440" xr2:uid="{1580F8C4-AF3E-5F4A-A010-F100369F5510}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
   <si>
     <t>FY21</t>
   </si>
@@ -184,6 +184,9 @@
   <si>
     <t>net_income_fraction</t>
   </si>
+  <si>
+    <t>FY22</t>
+  </si>
 </sst>
 </file>
 
@@ -325,13 +328,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
@@ -359,7 +364,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="37" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -404,15 +408,29 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="37" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="37" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="37" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="10" fillId="0" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="37" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="4" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="4" applyFont="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="5" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="5" fillId="2" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="5" applyFont="1"/>
+    <xf numFmtId="10" fontId="3" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="4" applyFont="1" applyFill="1"/>
+    <xf numFmtId="37" fontId="7" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -422,32 +440,18 @@
     <xf numFmtId="167" fontId="10" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="167" fontId="10" fillId="0" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="10" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="10" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="37" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="6">
     <cellStyle name="Comma 2" xfId="3" xr:uid="{C68451E4-A945-6545-A9E6-7D1F8818D189}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{3B161ADE-7E87-2F42-82D5-DBB5892DC2D1}"/>
+    <cellStyle name="Normal 3" xfId="4" xr:uid="{DD2E3D52-C969-CE43-B7C8-11BBAD8AA2DB}"/>
     <cellStyle name="Percent 2" xfId="2" xr:uid="{4AFB1077-5056-7F4F-8897-441B9281AF7F}"/>
+    <cellStyle name="Percent 3" xfId="5" xr:uid="{7226D3D1-F64C-0C4E-A00B-42110313B432}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -759,19 +763,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A109B183-BE6E-194B-93C2-5208D89F22E1}">
-  <dimension ref="A1:B28"/>
+  <dimension ref="A1:B29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="38" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="39" t="s">
+      <c r="B1" s="38" t="s">
         <v>47</v>
       </c>
     </row>
@@ -1015,6 +1019,14 @@
       </c>
       <c r="B28">
         <v>0.73</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>2023</v>
+      </c>
+      <c r="B29" s="58">
+        <v>0.77600000000000002</v>
       </c>
     </row>
   </sheetData>
@@ -1029,8 +1041,8 @@
   </sheetPr>
   <dimension ref="A1:AA122"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T32" sqref="T32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1429,9 +1441,9 @@
     <col min="16134" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="38"/>
-      <c r="B1" s="37" t="s">
+    <row r="1" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="37"/>
+      <c r="B1" s="36" t="s">
         <v>44</v>
       </c>
       <c r="C1" s="3"/>
@@ -1453,37 +1465,37 @@
       <c r="S1" s="3"/>
       <c r="T1" s="3"/>
     </row>
-    <row r="2" spans="1:25" ht="49" x14ac:dyDescent="0.2">
-      <c r="A2" s="36" t="s">
+    <row r="2" spans="1:24" ht="49" x14ac:dyDescent="0.2">
+      <c r="A2" s="35" t="s">
         <v>43</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="35"/>
+      <c r="C2" s="34"/>
       <c r="D2" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="E2" s="35"/>
-      <c r="F2" s="34" t="s">
+      <c r="E2" s="34"/>
+      <c r="F2" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="G2" s="34" t="s">
+      <c r="G2" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="H2" s="33" t="s">
+      <c r="H2" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="I2" s="33" t="s">
+      <c r="I2" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="J2" s="33" t="s">
+      <c r="J2" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="K2" s="33" t="s">
+      <c r="K2" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="L2" s="33" t="s">
+      <c r="L2" s="32" t="s">
         <v>34</v>
       </c>
       <c r="M2" s="9" t="s">
@@ -1492,1984 +1504,1985 @@
       <c r="N2" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="O2" s="33" t="s">
+      <c r="O2" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="P2" s="33" t="s">
+      <c r="P2" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="Q2" s="15"/>
-      <c r="R2" s="32" t="s">
+      <c r="Q2" s="14"/>
+      <c r="R2" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="S2" s="32" t="s">
+      <c r="S2" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="T2" s="32" t="s">
+      <c r="T2" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="U2" s="41"/>
-      <c r="V2" s="25"/>
-      <c r="W2" s="25"/>
-      <c r="X2" s="25"/>
-      <c r="Y2" s="42"/>
-    </row>
-    <row r="3" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+      <c r="U2" s="39"/>
+      <c r="V2" s="24"/>
+      <c r="W2" s="24"/>
+      <c r="X2" s="24"/>
+    </row>
+    <row r="3" spans="1:24" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
-      <c r="B3" s="22"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="31"/>
-      <c r="G3" s="31"/>
-      <c r="H3" s="28"/>
-      <c r="I3" s="28"/>
-      <c r="J3" s="28"/>
-      <c r="K3" s="28"/>
-      <c r="L3" s="30"/>
-      <c r="M3" s="29"/>
-      <c r="N3" s="29"/>
-      <c r="O3" s="28"/>
-      <c r="P3" s="28"/>
-      <c r="Q3" s="15"/>
-      <c r="R3" s="27"/>
-      <c r="S3" s="27"/>
-      <c r="T3" s="27"/>
-      <c r="U3" s="47"/>
-      <c r="V3" s="47"/>
-      <c r="W3" s="47"/>
-      <c r="X3" s="25"/>
-      <c r="Y3" s="42"/>
-    </row>
-    <row r="4" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="27"/>
+      <c r="I3" s="27"/>
+      <c r="J3" s="27"/>
+      <c r="K3" s="27"/>
+      <c r="L3" s="29"/>
+      <c r="M3" s="28"/>
+      <c r="N3" s="28"/>
+      <c r="O3" s="27"/>
+      <c r="P3" s="27"/>
+      <c r="Q3" s="14"/>
+      <c r="R3" s="26"/>
+      <c r="S3" s="26"/>
+      <c r="T3" s="26"/>
+      <c r="U3" s="54"/>
+      <c r="V3" s="54"/>
+      <c r="W3" s="54"/>
+      <c r="X3" s="24"/>
+    </row>
+    <row r="4" spans="1:24" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B4" s="8">
         <v>0.32500000000000001</v>
       </c>
-      <c r="C4" s="22"/>
-      <c r="D4" s="21">
+      <c r="C4" s="21"/>
+      <c r="D4" s="20">
         <v>6.5000000000000002E-2</v>
       </c>
-      <c r="E4" s="20"/>
-      <c r="F4" s="19">
+      <c r="E4" s="19"/>
+      <c r="F4" s="18">
         <v>0.69</v>
       </c>
-      <c r="G4" s="19">
+      <c r="G4" s="18">
         <v>0.31</v>
       </c>
-      <c r="H4" s="16">
+      <c r="H4" s="15">
         <f t="shared" ref="H4:H29" si="0">G4*R4</f>
         <v>0</v>
       </c>
-      <c r="I4" s="16" t="e">
+      <c r="I4" s="15" t="e">
         <f t="shared" ref="I4:I29" si="1">(H4/(1-$L4))-H4</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="J4" s="16">
+      <c r="J4" s="15">
         <f t="shared" ref="J4:J29" si="2">F4*R4</f>
         <v>0</v>
       </c>
-      <c r="K4" s="16" t="e">
+      <c r="K4" s="15" t="e">
         <f t="shared" ref="K4:K29" si="3">(J4/(1-$L4))-J4</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="L4" s="18" t="e">
+      <c r="L4" s="17" t="e">
         <f t="shared" ref="L4:L29" si="4">S4/(R4+S4)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="M4" s="17" t="e">
+      <c r="M4" s="16" t="e">
         <f t="shared" ref="M4:M29" si="5">(O4/O3)-1</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="N4" s="17" t="e">
+      <c r="N4" s="16" t="e">
         <f t="shared" ref="N4:N29" si="6">(P4/P3)-1</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="O4" s="16">
+      <c r="O4" s="15">
         <f>H4/AVERAGE(B4:C4)</f>
         <v>0</v>
       </c>
-      <c r="P4" s="16">
+      <c r="P4" s="15">
         <f>J4/(AVERAGE(D4:E4))</f>
         <v>0</v>
       </c>
-      <c r="Q4" s="15"/>
-      <c r="R4" s="14"/>
-      <c r="S4" s="14"/>
-      <c r="T4" s="14">
+      <c r="Q4" s="14"/>
+      <c r="R4" s="13"/>
+      <c r="S4" s="13"/>
+      <c r="T4" s="13">
         <f t="shared" ref="T4:T29" si="7">R4+S4</f>
         <v>0</v>
       </c>
-      <c r="U4" s="48" t="s">
+      <c r="U4" s="55" t="s">
         <v>46</v>
       </c>
-      <c r="V4" s="25"/>
-      <c r="W4" s="25"/>
-      <c r="X4" s="25"/>
-      <c r="Y4" s="42"/>
-    </row>
-    <row r="5" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+      <c r="V4" s="24"/>
+      <c r="W4" s="24"/>
+      <c r="X4" s="24"/>
+    </row>
+    <row r="5" spans="1:24" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>25</v>
       </c>
       <c r="B5" s="8">
         <v>0.32500000000000001</v>
       </c>
-      <c r="C5" s="22"/>
-      <c r="D5" s="21">
+      <c r="C5" s="21"/>
+      <c r="D5" s="20">
         <v>6.5000000000000002E-2</v>
       </c>
-      <c r="E5" s="20"/>
-      <c r="F5" s="19">
+      <c r="E5" s="19"/>
+      <c r="F5" s="18">
         <v>0.69</v>
       </c>
-      <c r="G5" s="19">
+      <c r="G5" s="18">
         <v>0.31</v>
       </c>
-      <c r="H5" s="16">
+      <c r="H5" s="15">
         <f t="shared" si="0"/>
         <v>66519.490000000005</v>
       </c>
-      <c r="I5" s="16">
+      <c r="I5" s="15">
         <f t="shared" si="1"/>
         <v>9276.4400000000023</v>
       </c>
-      <c r="J5" s="16">
+      <c r="J5" s="15">
         <f t="shared" si="2"/>
         <v>148059.50999999998</v>
       </c>
-      <c r="K5" s="16">
+      <c r="K5" s="15">
         <f t="shared" si="3"/>
         <v>20647.559999999998</v>
       </c>
-      <c r="L5" s="18">
+      <c r="L5" s="17">
         <f t="shared" si="4"/>
         <v>0.12238704637570909</v>
       </c>
-      <c r="M5" s="17" t="e">
+      <c r="M5" s="16" t="e">
         <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="N5" s="17" t="e">
+      <c r="N5" s="16" t="e">
         <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="O5" s="16">
+      <c r="O5" s="15">
         <f>H5/AVERAGE(B5:C5)</f>
         <v>204675.35384615386</v>
       </c>
-      <c r="P5" s="16">
+      <c r="P5" s="15">
         <f>J5/(AVERAGE(D5:E5))</f>
         <v>2277838.615384615</v>
       </c>
-      <c r="Q5" s="15"/>
-      <c r="R5" s="14">
+      <c r="Q5" s="14"/>
+      <c r="R5" s="13">
         <v>214579</v>
       </c>
-      <c r="S5" s="14">
+      <c r="S5" s="13">
         <v>29924</v>
       </c>
-      <c r="T5" s="14">
+      <c r="T5" s="13">
         <f t="shared" si="7"/>
         <v>244503</v>
       </c>
-      <c r="U5" s="49"/>
-      <c r="V5" s="25"/>
-      <c r="W5" s="25"/>
-      <c r="X5" s="25"/>
-      <c r="Y5" s="42"/>
-    </row>
-    <row r="6" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+      <c r="U5" s="56"/>
+      <c r="V5" s="24"/>
+      <c r="W5" s="24"/>
+      <c r="X5" s="24"/>
+    </row>
+    <row r="6" spans="1:24" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B6" s="8">
         <v>0.3</v>
       </c>
-      <c r="C6" s="22"/>
-      <c r="D6" s="21">
+      <c r="C6" s="21"/>
+      <c r="D6" s="20">
         <v>6.5000000000000002E-2</v>
       </c>
-      <c r="E6" s="20"/>
-      <c r="F6" s="19">
+      <c r="E6" s="19"/>
+      <c r="F6" s="18">
         <v>0.69</v>
       </c>
-      <c r="G6" s="19">
+      <c r="G6" s="18">
         <v>0.31</v>
       </c>
-      <c r="H6" s="16">
+      <c r="H6" s="15">
         <f t="shared" si="0"/>
         <v>65292.2</v>
       </c>
-      <c r="I6" s="16">
+      <c r="I6" s="15">
         <f t="shared" si="1"/>
         <v>11225.410000000003</v>
       </c>
-      <c r="J6" s="16">
+      <c r="J6" s="15">
         <f t="shared" si="2"/>
         <v>145327.79999999999</v>
       </c>
-      <c r="K6" s="16">
+      <c r="K6" s="15">
         <f t="shared" si="3"/>
         <v>24985.589999999997</v>
       </c>
-      <c r="L6" s="18">
+      <c r="L6" s="17">
         <f t="shared" si="4"/>
         <v>0.1467036150240448</v>
       </c>
-      <c r="M6" s="17">
+      <c r="M6" s="16">
         <f t="shared" si="5"/>
         <v>6.3345745234466788E-2</v>
       </c>
-      <c r="N6" s="17">
+      <c r="N6" s="16">
         <f t="shared" si="6"/>
         <v>-1.845008132203052E-2</v>
       </c>
-      <c r="O6" s="16">
+      <c r="O6" s="15">
         <f>H6/AVERAGE(B6:C6)</f>
         <v>217640.66666666666</v>
       </c>
-      <c r="P6" s="16">
+      <c r="P6" s="15">
         <f>J6/(AVERAGE(D6:E6))</f>
         <v>2235812.3076923075</v>
       </c>
-      <c r="Q6" s="15"/>
-      <c r="R6" s="14">
+      <c r="Q6" s="14"/>
+      <c r="R6" s="13">
         <v>210620</v>
       </c>
-      <c r="S6" s="14">
+      <c r="S6" s="13">
         <v>36211</v>
       </c>
-      <c r="T6" s="14">
+      <c r="T6" s="13">
         <f t="shared" si="7"/>
         <v>246831</v>
       </c>
-      <c r="U6" s="49"/>
-      <c r="V6" s="25"/>
-      <c r="W6" s="25"/>
-      <c r="X6" s="25"/>
-      <c r="Y6" s="42"/>
-    </row>
-    <row r="7" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+      <c r="U6" s="56"/>
+      <c r="V6" s="24"/>
+      <c r="W6" s="24"/>
+      <c r="X6" s="24"/>
+    </row>
+    <row r="7" spans="1:24" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B7" s="8">
         <v>0.29499999999999998</v>
       </c>
-      <c r="C7" s="22"/>
-      <c r="D7" s="21">
+      <c r="C7" s="21"/>
+      <c r="D7" s="20">
         <v>6.5000000000000002E-2</v>
       </c>
-      <c r="E7" s="20"/>
-      <c r="F7" s="19">
+      <c r="E7" s="19"/>
+      <c r="F7" s="18">
         <v>0.69</v>
       </c>
-      <c r="G7" s="19">
+      <c r="G7" s="18">
         <v>0.31</v>
       </c>
-      <c r="H7" s="16">
+      <c r="H7" s="15">
         <f t="shared" si="0"/>
         <v>66351.16</v>
       </c>
-      <c r="I7" s="16">
+      <c r="I7" s="15">
         <f t="shared" si="1"/>
         <v>7239.7400000000052</v>
       </c>
-      <c r="J7" s="16">
+      <c r="J7" s="15">
         <f t="shared" si="2"/>
         <v>147684.84</v>
       </c>
-      <c r="K7" s="16">
+      <c r="K7" s="15">
         <f t="shared" si="3"/>
         <v>16114.260000000009</v>
       </c>
-      <c r="L7" s="18">
+      <c r="L7" s="17">
         <f t="shared" si="4"/>
         <v>9.8378196217195332E-2</v>
       </c>
-      <c r="M7" s="17">
+      <c r="M7" s="16">
         <f t="shared" si="5"/>
         <v>3.3442829805143681E-2</v>
       </c>
-      <c r="N7" s="17">
+      <c r="N7" s="16">
         <f t="shared" si="6"/>
         <v>1.6218782641724605E-2</v>
       </c>
-      <c r="O7" s="16">
+      <c r="O7" s="15">
         <f t="shared" ref="O7:O29" si="8">H7/B7</f>
         <v>224919.18644067799</v>
       </c>
-      <c r="P7" s="16">
+      <c r="P7" s="15">
         <f t="shared" ref="P7:P29" si="9">J7/D7</f>
         <v>2272074.4615384615</v>
       </c>
-      <c r="Q7" s="15"/>
-      <c r="R7" s="14">
+      <c r="Q7" s="14"/>
+      <c r="R7" s="13">
         <v>214036</v>
       </c>
-      <c r="S7" s="14">
+      <c r="S7" s="13">
         <v>23354</v>
       </c>
-      <c r="T7" s="14">
+      <c r="T7" s="13">
         <f t="shared" si="7"/>
         <v>237390</v>
       </c>
-      <c r="U7" s="49"/>
-      <c r="V7" s="25"/>
-      <c r="W7" s="25"/>
-      <c r="X7" s="25"/>
-      <c r="Y7" s="42"/>
-    </row>
-    <row r="8" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+      <c r="U7" s="56"/>
+      <c r="V7" s="24"/>
+      <c r="W7" s="24"/>
+      <c r="X7" s="24"/>
+    </row>
+    <row r="8" spans="1:24" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B8" s="8">
         <v>0.28749999999999998</v>
       </c>
-      <c r="C8" s="22"/>
-      <c r="D8" s="21">
+      <c r="C8" s="21"/>
+      <c r="D8" s="20">
         <v>6.5000000000000002E-2</v>
       </c>
-      <c r="E8" s="20"/>
-      <c r="F8" s="19">
+      <c r="E8" s="19"/>
+      <c r="F8" s="18">
         <v>0.69</v>
       </c>
-      <c r="G8" s="19">
+      <c r="G8" s="18">
         <v>0.31</v>
       </c>
-      <c r="H8" s="16">
+      <c r="H8" s="15">
         <f t="shared" si="0"/>
         <v>72497.22</v>
       </c>
-      <c r="I8" s="16">
+      <c r="I8" s="15">
         <f t="shared" si="1"/>
         <v>6405.2200000000012</v>
       </c>
-      <c r="J8" s="16">
+      <c r="J8" s="15">
         <f t="shared" si="2"/>
         <v>161364.78</v>
       </c>
-      <c r="K8" s="16">
+      <c r="K8" s="15">
         <f t="shared" si="3"/>
         <v>14256.779999999999</v>
       </c>
-      <c r="L8" s="18">
+      <c r="L8" s="17">
         <f t="shared" si="4"/>
         <v>8.1178985085885808E-2</v>
       </c>
-      <c r="M8" s="17">
+      <c r="M8" s="16">
         <f t="shared" si="5"/>
         <v>0.12113264976960392</v>
       </c>
-      <c r="N8" s="17">
+      <c r="N8" s="16">
         <f t="shared" si="6"/>
         <v>9.2629277317834324E-2</v>
       </c>
-      <c r="O8" s="16">
+      <c r="O8" s="15">
         <f t="shared" si="8"/>
         <v>252164.24347826091</v>
       </c>
-      <c r="P8" s="16">
+      <c r="P8" s="15">
         <f t="shared" si="9"/>
         <v>2482535.076923077</v>
       </c>
-      <c r="Q8" s="15"/>
-      <c r="R8" s="14">
+      <c r="Q8" s="14"/>
+      <c r="R8" s="13">
         <v>233862</v>
       </c>
-      <c r="S8" s="14">
+      <c r="S8" s="13">
         <v>20662</v>
       </c>
-      <c r="T8" s="14">
+      <c r="T8" s="13">
         <f t="shared" si="7"/>
         <v>254524</v>
       </c>
-      <c r="U8" s="49"/>
-      <c r="V8" s="25"/>
-      <c r="W8" s="25"/>
-      <c r="X8" s="25"/>
-      <c r="Y8" s="42"/>
-    </row>
-    <row r="9" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+      <c r="U8" s="56"/>
+      <c r="V8" s="24"/>
+      <c r="W8" s="24"/>
+      <c r="X8" s="24"/>
+    </row>
+    <row r="9" spans="1:24" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B9" s="8">
         <v>0.27750000000000002</v>
       </c>
-      <c r="C9" s="22"/>
-      <c r="D9" s="21">
+      <c r="C9" s="21"/>
+      <c r="D9" s="20">
         <v>6.5000000000000002E-2</v>
       </c>
-      <c r="E9" s="20"/>
-      <c r="F9" s="19">
+      <c r="E9" s="19"/>
+      <c r="F9" s="18">
         <v>0.69</v>
       </c>
-      <c r="G9" s="19">
+      <c r="G9" s="18">
         <v>0.31</v>
       </c>
-      <c r="H9" s="16">
+      <c r="H9" s="15">
         <f t="shared" si="0"/>
         <v>78040.639999999999</v>
       </c>
-      <c r="I9" s="16">
+      <c r="I9" s="15">
         <f t="shared" si="1"/>
         <v>11897.179999999993</v>
       </c>
-      <c r="J9" s="16">
+      <c r="J9" s="15">
         <f t="shared" si="2"/>
         <v>173703.36</v>
       </c>
-      <c r="K9" s="16">
+      <c r="K9" s="15">
         <f t="shared" si="3"/>
         <v>26480.819999999978</v>
       </c>
-      <c r="L9" s="18">
+      <c r="L9" s="17">
         <f t="shared" si="4"/>
         <v>0.13228228124719946</v>
       </c>
-      <c r="M9" s="17">
+      <c r="M9" s="16">
         <f t="shared" si="5"/>
         <v>0.11525538931444945</v>
       </c>
-      <c r="N9" s="17">
+      <c r="N9" s="16">
         <f t="shared" si="6"/>
         <v>7.6463897512208057E-2</v>
       </c>
-      <c r="O9" s="16">
+      <c r="O9" s="15">
         <f t="shared" si="8"/>
         <v>281227.53153153148</v>
       </c>
-      <c r="P9" s="16">
+      <c r="P9" s="15">
         <f t="shared" si="9"/>
         <v>2672359.3846153845</v>
       </c>
-      <c r="Q9" s="15"/>
-      <c r="R9" s="14">
+      <c r="Q9" s="14"/>
+      <c r="R9" s="13">
         <v>251744</v>
       </c>
-      <c r="S9" s="14">
+      <c r="S9" s="13">
         <v>38378</v>
       </c>
-      <c r="T9" s="14">
+      <c r="T9" s="13">
         <f t="shared" si="7"/>
         <v>290122</v>
       </c>
-      <c r="U9" s="49"/>
-      <c r="V9" s="25"/>
-      <c r="W9" s="25"/>
-      <c r="X9" s="25"/>
-      <c r="Y9" s="42"/>
-    </row>
-    <row r="10" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+      <c r="U9" s="56"/>
+      <c r="V9" s="24"/>
+      <c r="W9" s="24"/>
+      <c r="X9" s="24"/>
+    </row>
+    <row r="10" spans="1:24" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="26">
+      <c r="B10" s="25">
         <v>0.26500000000000001</v>
       </c>
-      <c r="C10" s="22"/>
-      <c r="D10" s="21">
+      <c r="C10" s="21"/>
+      <c r="D10" s="20">
         <v>6.5000000000000002E-2</v>
       </c>
-      <c r="E10" s="20"/>
-      <c r="F10" s="19">
+      <c r="E10" s="19"/>
+      <c r="F10" s="18">
         <v>0.69</v>
       </c>
-      <c r="G10" s="19">
+      <c r="G10" s="18">
         <v>0.31</v>
       </c>
-      <c r="H10" s="16">
+      <c r="H10" s="15">
         <f t="shared" si="0"/>
         <v>85390.43</v>
       </c>
-      <c r="I10" s="16">
+      <c r="I10" s="15">
         <f t="shared" si="1"/>
         <v>11935.929999999993</v>
       </c>
-      <c r="J10" s="16">
+      <c r="J10" s="15">
         <f t="shared" si="2"/>
         <v>190062.56999999998</v>
       </c>
-      <c r="K10" s="16">
+      <c r="K10" s="15">
         <f t="shared" si="3"/>
         <v>26567.069999999978</v>
       </c>
-      <c r="L10" s="18">
+      <c r="L10" s="17">
         <f t="shared" si="4"/>
         <v>0.12263820407955255</v>
       </c>
-      <c r="M10" s="17">
+      <c r="M10" s="16">
         <f t="shared" si="5"/>
         <v>0.1457912245683548</v>
       </c>
-      <c r="N10" s="17">
+      <c r="N10" s="16">
         <f t="shared" si="6"/>
         <v>9.4179007245455582E-2</v>
       </c>
-      <c r="O10" s="16">
+      <c r="O10" s="15">
         <f t="shared" si="8"/>
         <v>322228.03773584904</v>
       </c>
-      <c r="P10" s="16">
+      <c r="P10" s="15">
         <f t="shared" si="9"/>
         <v>2924039.538461538</v>
       </c>
-      <c r="Q10" s="15"/>
-      <c r="R10" s="14">
+      <c r="Q10" s="14"/>
+      <c r="R10" s="13">
         <v>275453</v>
       </c>
-      <c r="S10" s="14">
+      <c r="S10" s="13">
         <v>38503</v>
       </c>
-      <c r="T10" s="14">
+      <c r="T10" s="13">
         <f t="shared" si="7"/>
         <v>313956</v>
       </c>
-      <c r="U10" s="49"/>
-      <c r="V10" s="25"/>
-      <c r="W10" s="25"/>
-      <c r="X10" s="25"/>
-      <c r="Y10" s="42"/>
-    </row>
-    <row r="11" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+      <c r="U10" s="56"/>
+      <c r="V10" s="24"/>
+      <c r="W10" s="24"/>
+      <c r="X10" s="24"/>
+    </row>
+    <row r="11" spans="1:24" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="26">
+      <c r="B11" s="25">
         <v>0.2525</v>
       </c>
-      <c r="C11" s="22"/>
-      <c r="D11" s="21">
+      <c r="C11" s="21"/>
+      <c r="D11" s="20">
         <v>6.5000000000000002E-2</v>
       </c>
-      <c r="E11" s="20"/>
-      <c r="F11" s="19">
+      <c r="E11" s="19"/>
+      <c r="F11" s="18">
         <v>0.69</v>
       </c>
-      <c r="G11" s="19">
+      <c r="G11" s="18">
         <v>0.31</v>
       </c>
-      <c r="H11" s="16">
+      <c r="H11" s="15">
         <f t="shared" si="0"/>
         <v>84867.46</v>
       </c>
-      <c r="I11" s="16">
+      <c r="I11" s="15">
         <f t="shared" si="1"/>
         <v>6830.5399999999936</v>
       </c>
-      <c r="J11" s="16">
+      <c r="J11" s="15">
         <f t="shared" si="2"/>
         <v>188898.53999999998</v>
       </c>
-      <c r="K11" s="16">
+      <c r="K11" s="15">
         <f t="shared" si="3"/>
         <v>15203.459999999992</v>
       </c>
-      <c r="L11" s="18">
+      <c r="L11" s="17">
         <f t="shared" si="4"/>
         <v>7.4489519945909397E-2</v>
       </c>
-      <c r="M11" s="17">
+      <c r="M11" s="16">
         <f t="shared" si="5"/>
         <v>4.3077302760281322E-2</v>
       </c>
-      <c r="N11" s="17">
+      <c r="N11" s="16">
         <f t="shared" si="6"/>
         <v>-6.1244568038830716E-3</v>
       </c>
-      <c r="O11" s="16">
+      <c r="O11" s="15">
         <f t="shared" si="8"/>
         <v>336108.75247524754</v>
       </c>
-      <c r="P11" s="16">
+      <c r="P11" s="15">
         <f t="shared" si="9"/>
         <v>2906131.384615384</v>
       </c>
-      <c r="Q11" s="15"/>
-      <c r="R11" s="14">
+      <c r="Q11" s="14"/>
+      <c r="R11" s="13">
         <v>273766</v>
       </c>
-      <c r="S11" s="14">
+      <c r="S11" s="13">
         <v>22034</v>
       </c>
-      <c r="T11" s="14">
+      <c r="T11" s="13">
         <f t="shared" si="7"/>
         <v>295800</v>
       </c>
-      <c r="U11" s="49"/>
-      <c r="V11" s="25"/>
-      <c r="W11" s="25"/>
-      <c r="X11" s="25"/>
-      <c r="Y11" s="42"/>
-    </row>
-    <row r="12" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+      <c r="U11" s="56"/>
+      <c r="V11" s="24"/>
+      <c r="W11" s="24"/>
+      <c r="X11" s="24"/>
+    </row>
+    <row r="12" spans="1:24" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="26">
+      <c r="B12" s="25">
         <v>0.24</v>
       </c>
-      <c r="C12" s="22"/>
-      <c r="D12" s="21">
+      <c r="C12" s="21"/>
+      <c r="D12" s="20">
         <v>6.5000000000000002E-2</v>
       </c>
-      <c r="E12" s="20"/>
-      <c r="F12" s="19">
+      <c r="E12" s="19"/>
+      <c r="F12" s="18">
         <v>0.69</v>
       </c>
-      <c r="G12" s="19">
+      <c r="G12" s="18">
         <v>0.31</v>
       </c>
-      <c r="H12" s="16">
+      <c r="H12" s="15">
         <f t="shared" si="0"/>
         <v>74004.44</v>
       </c>
-      <c r="I12" s="16">
+      <c r="I12" s="15">
         <f t="shared" si="1"/>
         <v>14682.840000000011</v>
       </c>
-      <c r="J12" s="16">
+      <c r="J12" s="15">
         <f t="shared" si="2"/>
         <v>164719.56</v>
       </c>
-      <c r="K12" s="16">
+      <c r="K12" s="15">
         <f t="shared" si="3"/>
         <v>32681.160000000003</v>
       </c>
-      <c r="L12" s="18">
+      <c r="L12" s="17">
         <f t="shared" si="4"/>
         <v>0.16555745085428261</v>
       </c>
-      <c r="M12" s="17">
+      <c r="M12" s="16">
         <f t="shared" si="5"/>
         <v>-8.2583148869228906E-2</v>
       </c>
-      <c r="N12" s="17">
+      <c r="N12" s="16">
         <f t="shared" si="6"/>
         <v>-0.12799982466778181</v>
       </c>
-      <c r="O12" s="16">
+      <c r="O12" s="15">
         <f t="shared" si="8"/>
         <v>308351.83333333337</v>
       </c>
-      <c r="P12" s="16">
+      <c r="P12" s="15">
         <f t="shared" si="9"/>
         <v>2534147.076923077</v>
       </c>
-      <c r="Q12" s="15"/>
-      <c r="R12" s="14">
+      <c r="Q12" s="14"/>
+      <c r="R12" s="13">
         <v>238724</v>
       </c>
-      <c r="S12" s="14">
+      <c r="S12" s="13">
         <v>47364</v>
       </c>
-      <c r="T12" s="14">
+      <c r="T12" s="13">
         <f t="shared" si="7"/>
         <v>286088</v>
       </c>
-      <c r="U12" s="49"/>
-      <c r="V12" s="25"/>
-      <c r="W12" s="25"/>
-      <c r="X12" s="25"/>
-      <c r="Y12" s="42"/>
-    </row>
-    <row r="13" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+      <c r="U12" s="56"/>
+      <c r="V12" s="24"/>
+      <c r="W12" s="24"/>
+      <c r="X12" s="24"/>
+    </row>
+    <row r="13" spans="1:24" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="26">
+      <c r="B13" s="25">
         <v>0.23</v>
       </c>
-      <c r="C13" s="22"/>
-      <c r="D13" s="21">
+      <c r="C13" s="21"/>
+      <c r="D13" s="20">
         <v>6.5000000000000002E-2</v>
       </c>
-      <c r="E13" s="20"/>
-      <c r="F13" s="19">
+      <c r="E13" s="19"/>
+      <c r="F13" s="18">
         <v>0.69</v>
       </c>
-      <c r="G13" s="19">
+      <c r="G13" s="18">
         <v>0.31</v>
       </c>
-      <c r="H13" s="16">
+      <c r="H13" s="15">
         <f t="shared" si="0"/>
         <v>83681.710000000006</v>
       </c>
-      <c r="I13" s="16">
+      <c r="I13" s="15">
         <f t="shared" si="1"/>
         <v>12164.089999999997</v>
       </c>
-      <c r="J13" s="16">
+      <c r="J13" s="15">
         <f t="shared" si="2"/>
         <v>186259.28999999998</v>
       </c>
-      <c r="K13" s="16">
+      <c r="K13" s="15">
         <f t="shared" si="3"/>
         <v>27074.910000000003</v>
       </c>
-      <c r="L13" s="18">
+      <c r="L13" s="17">
         <f t="shared" si="4"/>
         <v>0.12691312504042954</v>
       </c>
-      <c r="M13" s="17">
+      <c r="M13" s="16">
         <f t="shared" si="5"/>
         <v>0.17992981525691287</v>
       </c>
-      <c r="N13" s="17">
+      <c r="N13" s="16">
         <f t="shared" si="6"/>
         <v>0.13076607295454146</v>
       </c>
-      <c r="O13" s="16">
+      <c r="O13" s="15">
         <f t="shared" si="8"/>
         <v>363833.52173913043</v>
       </c>
-      <c r="P13" s="16">
+      <c r="P13" s="15">
         <f t="shared" si="9"/>
         <v>2865527.538461538</v>
       </c>
-      <c r="Q13" s="15"/>
-      <c r="R13" s="14">
+      <c r="Q13" s="14"/>
+      <c r="R13" s="13">
         <v>269941</v>
       </c>
-      <c r="S13" s="14">
+      <c r="S13" s="13">
         <v>39239</v>
       </c>
-      <c r="T13" s="14">
+      <c r="T13" s="13">
         <f t="shared" si="7"/>
         <v>309180</v>
       </c>
-      <c r="U13" s="49"/>
-      <c r="V13" s="25"/>
-      <c r="W13" s="25"/>
-      <c r="X13" s="25"/>
-      <c r="Y13" s="42"/>
-    </row>
-    <row r="14" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+      <c r="U13" s="56"/>
+      <c r="V13" s="24"/>
+      <c r="W13" s="24"/>
+      <c r="X13" s="24"/>
+    </row>
+    <row r="14" spans="1:24" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="26">
+      <c r="B14" s="25">
         <v>0.21</v>
       </c>
-      <c r="C14" s="22"/>
-      <c r="D14" s="21">
+      <c r="C14" s="21"/>
+      <c r="D14" s="20">
         <v>6.5000000000000002E-2</v>
       </c>
-      <c r="E14" s="20"/>
-      <c r="F14" s="19">
+      <c r="E14" s="19"/>
+      <c r="F14" s="18">
         <v>0.69</v>
       </c>
-      <c r="G14" s="19">
+      <c r="G14" s="18">
         <v>0.31</v>
       </c>
-      <c r="H14" s="16">
+      <c r="H14" s="15">
         <f t="shared" si="0"/>
         <v>101260.88</v>
       </c>
-      <c r="I14" s="16">
+      <c r="I14" s="15">
         <f t="shared" si="1"/>
         <v>16370.479999999996</v>
       </c>
-      <c r="J14" s="16">
+      <c r="J14" s="15">
         <f t="shared" si="2"/>
         <v>225387.12</v>
       </c>
-      <c r="K14" s="16">
+      <c r="K14" s="15">
         <f t="shared" si="3"/>
         <v>36437.51999999999</v>
       </c>
-      <c r="L14" s="18">
+      <c r="L14" s="17">
         <f t="shared" si="4"/>
         <v>0.13916765053128691</v>
       </c>
-      <c r="M14" s="17">
+      <c r="M14" s="16">
         <f t="shared" si="5"/>
         <v>0.32531676675026522</v>
       </c>
-      <c r="N14" s="17">
+      <c r="N14" s="16">
         <f t="shared" si="6"/>
         <v>0.21007183051111178</v>
       </c>
-      <c r="O14" s="16">
+      <c r="O14" s="15">
         <f t="shared" si="8"/>
         <v>482194.66666666669</v>
       </c>
-      <c r="P14" s="16">
+      <c r="P14" s="15">
         <f t="shared" si="9"/>
         <v>3467494.1538461535</v>
       </c>
-      <c r="Q14" s="15"/>
-      <c r="R14" s="14">
+      <c r="Q14" s="14"/>
+      <c r="R14" s="13">
         <v>326648</v>
       </c>
-      <c r="S14" s="14">
+      <c r="S14" s="13">
         <v>52808</v>
       </c>
-      <c r="T14" s="14">
+      <c r="T14" s="13">
         <f t="shared" si="7"/>
         <v>379456</v>
       </c>
-      <c r="U14" s="49"/>
-      <c r="V14" s="25"/>
-      <c r="W14" s="25"/>
-      <c r="X14" s="25"/>
-      <c r="Y14" s="42"/>
-    </row>
-    <row r="15" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+      <c r="U14" s="56"/>
+      <c r="V14" s="24"/>
+      <c r="W14" s="24"/>
+      <c r="X14" s="24"/>
+    </row>
+    <row r="15" spans="1:24" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="26">
+      <c r="B15" s="25">
         <v>0.19</v>
       </c>
-      <c r="C15" s="22"/>
-      <c r="D15" s="21">
+      <c r="C15" s="21"/>
+      <c r="D15" s="20">
         <v>6.5000000000000002E-2</v>
       </c>
-      <c r="E15" s="20"/>
-      <c r="F15" s="19">
+      <c r="E15" s="19"/>
+      <c r="F15" s="18">
         <v>0.71</v>
       </c>
-      <c r="G15" s="19">
+      <c r="G15" s="18">
         <v>0.28999999999999998</v>
       </c>
-      <c r="H15" s="16">
+      <c r="H15" s="15">
         <f t="shared" si="0"/>
         <v>113234.26999999999</v>
       </c>
-      <c r="I15" s="16">
+      <c r="I15" s="15">
         <f t="shared" si="1"/>
         <v>7261.8899999999994</v>
       </c>
-      <c r="J15" s="16">
+      <c r="J15" s="15">
         <f t="shared" si="2"/>
         <v>277228.73</v>
       </c>
-      <c r="K15" s="16">
+      <c r="K15" s="15">
         <f t="shared" si="3"/>
         <v>17779.109999999986</v>
       </c>
-      <c r="L15" s="18">
+      <c r="L15" s="17">
         <f t="shared" si="4"/>
         <v>6.0266567830875271E-2</v>
       </c>
-      <c r="M15" s="17">
+      <c r="M15" s="16">
         <f t="shared" si="5"/>
         <v>0.23595278692131894</v>
       </c>
-      <c r="N15" s="17">
+      <c r="N15" s="16">
         <f t="shared" si="6"/>
         <v>0.23001141325200836</v>
       </c>
-      <c r="O15" s="16">
+      <c r="O15" s="15">
         <f t="shared" si="8"/>
         <v>595969.84210526315</v>
       </c>
-      <c r="P15" s="16">
+      <c r="P15" s="15">
         <f t="shared" si="9"/>
         <v>4265057.384615384</v>
       </c>
-      <c r="Q15" s="15"/>
-      <c r="R15" s="14">
+      <c r="Q15" s="14"/>
+      <c r="R15" s="13">
         <v>390463</v>
       </c>
-      <c r="S15" s="14">
+      <c r="S15" s="13">
         <v>25041</v>
       </c>
-      <c r="T15" s="14">
+      <c r="T15" s="13">
         <f t="shared" si="7"/>
         <v>415504</v>
       </c>
-      <c r="U15" s="49"/>
-      <c r="V15" s="25"/>
-      <c r="W15" s="25"/>
-      <c r="X15" s="25"/>
-      <c r="Y15" s="42"/>
-    </row>
-    <row r="16" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+      <c r="U15" s="56"/>
+      <c r="V15" s="24"/>
+      <c r="W15" s="24"/>
+      <c r="X15" s="24"/>
+    </row>
+    <row r="16" spans="1:24" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="23">
+      <c r="B16" s="22">
         <v>0.16650000000000001</v>
       </c>
-      <c r="C16" s="22"/>
-      <c r="D16" s="21">
+      <c r="C16" s="21"/>
+      <c r="D16" s="20">
         <v>6.5000000000000002E-2</v>
       </c>
-      <c r="E16" s="20"/>
-      <c r="F16" s="19">
+      <c r="E16" s="19"/>
+      <c r="F16" s="18">
         <v>0.75</v>
       </c>
-      <c r="G16" s="19">
+      <c r="G16" s="18">
         <v>0.25</v>
       </c>
-      <c r="H16" s="16">
+      <c r="H16" s="15">
         <f t="shared" si="0"/>
         <v>100477.75</v>
       </c>
-      <c r="I16" s="16">
+      <c r="I16" s="15">
         <f t="shared" si="1"/>
         <v>8611.75</v>
       </c>
-      <c r="J16" s="16">
+      <c r="J16" s="15">
         <f t="shared" si="2"/>
         <v>301433.25</v>
       </c>
-      <c r="K16" s="16">
+      <c r="K16" s="15">
         <f t="shared" si="3"/>
         <v>25835.25</v>
       </c>
-      <c r="L16" s="18">
+      <c r="L16" s="17">
         <f t="shared" si="4"/>
         <v>7.8942061334958916E-2</v>
       </c>
-      <c r="M16" s="17">
+      <c r="M16" s="16">
         <f t="shared" si="5"/>
         <v>1.258474394981568E-2</v>
       </c>
-      <c r="N16" s="17">
+      <c r="N16" s="16">
         <f t="shared" si="6"/>
         <v>8.7308844216831494E-2</v>
       </c>
-      <c r="O16" s="16">
+      <c r="O16" s="15">
         <f t="shared" si="8"/>
         <v>603469.96996996994</v>
       </c>
-      <c r="P16" s="16">
+      <c r="P16" s="15">
         <f t="shared" si="9"/>
         <v>4637434.615384615</v>
       </c>
-      <c r="Q16" s="15"/>
-      <c r="R16" s="14">
+      <c r="Q16" s="14"/>
+      <c r="R16" s="13">
         <v>401911</v>
       </c>
-      <c r="S16" s="14">
+      <c r="S16" s="13">
         <v>34447</v>
       </c>
-      <c r="T16" s="14">
+      <c r="T16" s="13">
         <f t="shared" si="7"/>
         <v>436358</v>
       </c>
-      <c r="U16" s="49"/>
-      <c r="V16" s="25"/>
-      <c r="W16" s="25"/>
-      <c r="X16" s="25"/>
-      <c r="Y16" s="42"/>
-    </row>
-    <row r="17" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+      <c r="U16" s="56"/>
+      <c r="V16" s="24"/>
+      <c r="W16" s="24"/>
+      <c r="X16" s="24"/>
+    </row>
+    <row r="17" spans="1:24" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="23">
+      <c r="B17" s="22">
         <v>0.154</v>
       </c>
-      <c r="C17" s="22"/>
-      <c r="D17" s="21">
+      <c r="C17" s="21"/>
+      <c r="D17" s="20">
         <v>6.5000000000000002E-2</v>
       </c>
-      <c r="E17" s="20"/>
-      <c r="F17" s="19">
+      <c r="E17" s="19"/>
+      <c r="F17" s="18">
         <v>0.75</v>
       </c>
-      <c r="G17" s="19">
+      <c r="G17" s="18">
         <v>0.25</v>
       </c>
-      <c r="H17" s="16">
+      <c r="H17" s="15">
         <f t="shared" si="0"/>
         <v>94033.25</v>
       </c>
-      <c r="I17" s="16">
+      <c r="I17" s="15">
         <f t="shared" si="1"/>
         <v>5673.5</v>
       </c>
-      <c r="J17" s="16">
+      <c r="J17" s="15">
         <f t="shared" si="2"/>
         <v>282099.75</v>
       </c>
-      <c r="K17" s="16">
+      <c r="K17" s="15">
         <f t="shared" si="3"/>
         <v>17020.5</v>
       </c>
-      <c r="L17" s="18">
+      <c r="L17" s="17">
         <f t="shared" si="4"/>
         <v>5.6901864718286378E-2</v>
       </c>
-      <c r="M17" s="17">
+      <c r="M17" s="16">
         <f t="shared" si="5"/>
         <v>1.1824199820422931E-2</v>
       </c>
-      <c r="N17" s="17">
+      <c r="N17" s="16">
         <f t="shared" si="6"/>
         <v>-6.413857794387301E-2</v>
       </c>
-      <c r="O17" s="16">
+      <c r="O17" s="15">
         <f t="shared" si="8"/>
         <v>610605.51948051946</v>
       </c>
-      <c r="P17" s="16">
+      <c r="P17" s="15">
         <f t="shared" si="9"/>
         <v>4339996.153846154</v>
       </c>
-      <c r="Q17" s="15"/>
-      <c r="R17" s="14">
+      <c r="Q17" s="14"/>
+      <c r="R17" s="13">
         <v>376133</v>
       </c>
-      <c r="S17" s="14">
+      <c r="S17" s="13">
         <v>22694</v>
       </c>
-      <c r="T17" s="14">
+      <c r="T17" s="13">
         <f t="shared" si="7"/>
         <v>398827</v>
       </c>
-      <c r="U17" s="49"/>
-      <c r="V17" s="25"/>
-      <c r="W17" s="25"/>
-      <c r="X17" s="25"/>
-      <c r="Y17" s="42"/>
-    </row>
-    <row r="18" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+      <c r="U17" s="56"/>
+      <c r="V17" s="24"/>
+      <c r="W17" s="24"/>
+      <c r="X17" s="24"/>
+    </row>
+    <row r="18" spans="1:24" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B18" s="23">
+      <c r="B18" s="22">
         <v>0.14149999999999999</v>
       </c>
-      <c r="C18" s="22"/>
-      <c r="D18" s="21">
+      <c r="C18" s="21"/>
+      <c r="D18" s="20">
         <v>6.4500000000000002E-2</v>
       </c>
-      <c r="E18" s="20"/>
-      <c r="F18" s="19">
+      <c r="E18" s="19"/>
+      <c r="F18" s="18">
         <v>0.75</v>
       </c>
-      <c r="G18" s="19">
+      <c r="G18" s="18">
         <v>0.25</v>
       </c>
-      <c r="H18" s="16">
+      <c r="H18" s="15">
         <f t="shared" si="0"/>
         <v>91768.5</v>
       </c>
-      <c r="I18" s="16">
+      <c r="I18" s="15">
         <f t="shared" si="1"/>
         <v>4729</v>
       </c>
-      <c r="J18" s="16">
+      <c r="J18" s="15">
         <f t="shared" si="2"/>
         <v>275305.5</v>
       </c>
-      <c r="K18" s="16">
+      <c r="K18" s="15">
         <f t="shared" si="3"/>
         <v>14187</v>
       </c>
-      <c r="L18" s="18">
+      <c r="L18" s="17">
         <f t="shared" si="4"/>
         <v>4.9006450944324979E-2</v>
       </c>
-      <c r="M18" s="17">
+      <c r="M18" s="16">
         <f t="shared" si="5"/>
         <v>6.2127044960480049E-2</v>
       </c>
-      <c r="N18" s="17">
+      <c r="N18" s="16">
         <f t="shared" si="6"/>
         <v>-1.6519329907982327E-2</v>
       </c>
-      <c r="O18" s="16">
+      <c r="O18" s="15">
         <f t="shared" si="8"/>
         <v>648540.63604240294</v>
       </c>
-      <c r="P18" s="16">
+      <c r="P18" s="15">
         <f t="shared" si="9"/>
         <v>4268302.3255813951</v>
       </c>
-      <c r="Q18" s="15"/>
-      <c r="R18" s="14">
+      <c r="Q18" s="14"/>
+      <c r="R18" s="13">
         <v>367074</v>
       </c>
-      <c r="S18" s="14">
+      <c r="S18" s="13">
         <v>18916</v>
       </c>
-      <c r="T18" s="14">
+      <c r="T18" s="13">
         <f t="shared" si="7"/>
         <v>385990</v>
       </c>
-      <c r="U18" s="49"/>
-      <c r="V18" s="25"/>
-      <c r="W18" s="25"/>
-      <c r="X18" s="25"/>
-      <c r="Y18" s="42"/>
-    </row>
-    <row r="19" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+      <c r="U18" s="56"/>
+      <c r="V18" s="24"/>
+      <c r="W18" s="24"/>
+      <c r="X18" s="24"/>
+    </row>
+    <row r="19" spans="1:24" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B19" s="23">
+      <c r="B19" s="22">
         <v>0.14149999999999999</v>
       </c>
-      <c r="C19" s="22"/>
-      <c r="D19" s="21">
+      <c r="C19" s="21"/>
+      <c r="D19" s="20">
         <v>6.4500000000000002E-2</v>
       </c>
-      <c r="E19" s="20"/>
-      <c r="F19" s="19">
+      <c r="E19" s="19"/>
+      <c r="F19" s="18">
         <v>0.74</v>
       </c>
-      <c r="G19" s="19">
+      <c r="G19" s="18">
         <v>0.26</v>
       </c>
-      <c r="H19" s="16">
+      <c r="H19" s="15">
         <f t="shared" si="0"/>
         <v>85611.5</v>
       </c>
-      <c r="I19" s="16">
+      <c r="I19" s="15">
         <f t="shared" si="1"/>
         <v>9211.2799999999988</v>
       </c>
-      <c r="J19" s="16">
+      <c r="J19" s="15">
         <f t="shared" si="2"/>
         <v>243663.5</v>
       </c>
-      <c r="K19" s="16">
+      <c r="K19" s="15">
         <f t="shared" si="3"/>
         <v>26216.719999999972</v>
       </c>
-      <c r="L19" s="18">
+      <c r="L19" s="17">
         <f t="shared" si="4"/>
         <v>9.7142058058200781E-2</v>
       </c>
-      <c r="M19" s="17">
+      <c r="M19" s="16">
         <f t="shared" si="5"/>
         <v>-6.7092738793812723E-2</v>
       </c>
-      <c r="N19" s="17">
+      <c r="N19" s="16">
         <f t="shared" si="6"/>
         <v>-0.11493413680438636</v>
       </c>
-      <c r="O19" s="16">
+      <c r="O19" s="15">
         <f t="shared" si="8"/>
         <v>605028.26855123683</v>
       </c>
-      <c r="P19" s="16">
+      <c r="P19" s="15">
         <f t="shared" si="9"/>
         <v>3777728.6821705424</v>
       </c>
-      <c r="Q19" s="15"/>
-      <c r="R19" s="14">
+      <c r="Q19" s="14"/>
+      <c r="R19" s="13">
         <v>329275</v>
       </c>
-      <c r="S19" s="14">
+      <c r="S19" s="13">
         <v>35428</v>
       </c>
-      <c r="T19" s="14">
+      <c r="T19" s="13">
         <f t="shared" si="7"/>
         <v>364703</v>
       </c>
-      <c r="U19" s="49"/>
-      <c r="V19" s="43"/>
-      <c r="W19" s="44"/>
-      <c r="X19" s="25"/>
-      <c r="Y19" s="42"/>
-    </row>
-    <row r="20" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+      <c r="U19" s="56"/>
+      <c r="V19" s="3"/>
+      <c r="W19" s="40"/>
+      <c r="X19" s="24"/>
+    </row>
+    <row r="20" spans="1:24" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B20" s="23">
+      <c r="B20" s="22">
         <v>0.14149999999999999</v>
       </c>
-      <c r="C20" s="22"/>
-      <c r="D20" s="21">
+      <c r="C20" s="21"/>
+      <c r="D20" s="20">
         <v>6.4500000000000002E-2</v>
       </c>
-      <c r="E20" s="20"/>
-      <c r="F20" s="19">
+      <c r="E20" s="19"/>
+      <c r="F20" s="18">
         <v>0.74</v>
       </c>
-      <c r="G20" s="19">
+      <c r="G20" s="18">
         <v>0.26</v>
       </c>
-      <c r="H20" s="16">
+      <c r="H20" s="15">
         <f t="shared" si="0"/>
         <v>87098.96</v>
       </c>
-      <c r="I20" s="16">
+      <c r="I20" s="15">
         <f t="shared" si="1"/>
         <v>10907</v>
       </c>
-      <c r="J20" s="16">
+      <c r="J20" s="15">
         <f t="shared" si="2"/>
         <v>247897.04</v>
       </c>
-      <c r="K20" s="16">
+      <c r="K20" s="15">
         <f t="shared" si="3"/>
         <v>31043.000000000029</v>
       </c>
-      <c r="L20" s="18">
+      <c r="L20" s="17">
         <f t="shared" si="4"/>
         <v>0.11128915017005088</v>
       </c>
-      <c r="M20" s="17">
+      <c r="M20" s="16">
         <f t="shared" si="5"/>
         <v>1.7374534963176869E-2</v>
       </c>
-      <c r="N20" s="17">
+      <c r="N20" s="16">
         <f t="shared" si="6"/>
         <v>1.7374534963176869E-2</v>
       </c>
-      <c r="O20" s="16">
+      <c r="O20" s="15">
         <f t="shared" si="8"/>
         <v>615540.35335689061</v>
       </c>
-      <c r="P20" s="16">
+      <c r="P20" s="15">
         <f t="shared" si="9"/>
         <v>3843364.9612403102</v>
       </c>
-      <c r="Q20" s="15"/>
-      <c r="R20" s="14">
+      <c r="Q20" s="14"/>
+      <c r="R20" s="13">
         <v>334996</v>
       </c>
-      <c r="S20" s="14">
+      <c r="S20" s="13">
         <v>41950</v>
       </c>
-      <c r="T20" s="14">
+      <c r="T20" s="13">
         <f t="shared" si="7"/>
         <v>376946</v>
       </c>
-      <c r="U20" s="49"/>
-      <c r="V20" s="42"/>
-      <c r="W20" s="42"/>
-      <c r="X20" s="25"/>
-      <c r="Y20" s="42"/>
-    </row>
-    <row r="21" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+      <c r="U20" s="56"/>
+      <c r="X20" s="24"/>
+    </row>
+    <row r="21" spans="1:24" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B21" s="23">
+      <c r="B21" s="22">
         <v>0.14149999999999999</v>
       </c>
-      <c r="C21" s="22"/>
-      <c r="D21" s="21">
+      <c r="C21" s="21"/>
+      <c r="D21" s="20">
         <v>6.4500000000000002E-2</v>
       </c>
-      <c r="E21" s="20"/>
-      <c r="F21" s="19">
+      <c r="E21" s="19"/>
+      <c r="F21" s="18">
         <v>0.74</v>
       </c>
-      <c r="G21" s="19">
+      <c r="G21" s="18">
         <v>0.26</v>
       </c>
-      <c r="H21" s="16">
+      <c r="H21" s="15">
         <f t="shared" si="0"/>
         <v>96249.14</v>
       </c>
-      <c r="I21" s="16">
+      <c r="I21" s="15">
         <f t="shared" si="1"/>
         <v>4991.2200000000012</v>
       </c>
-      <c r="J21" s="16">
+      <c r="J21" s="15">
         <f t="shared" si="2"/>
         <v>273939.86</v>
       </c>
-      <c r="K21" s="16">
+      <c r="K21" s="15">
         <f t="shared" si="3"/>
         <v>14205.780000000028</v>
       </c>
-      <c r="L21" s="18">
+      <c r="L21" s="17">
         <f t="shared" si="4"/>
         <v>4.9300693912980947E-2</v>
       </c>
-      <c r="M21" s="17">
+      <c r="M21" s="16">
         <f t="shared" si="5"/>
         <v>0.10505498573117289</v>
       </c>
-      <c r="N21" s="17">
+      <c r="N21" s="16">
         <f t="shared" si="6"/>
         <v>0.10505498573117267</v>
       </c>
-      <c r="O21" s="16">
+      <c r="O21" s="15">
         <f t="shared" si="8"/>
         <v>680205.93639575981</v>
       </c>
-      <c r="P21" s="16">
+      <c r="P21" s="15">
         <f t="shared" si="9"/>
         <v>4247129.6124031004</v>
       </c>
-      <c r="Q21" s="15"/>
-      <c r="R21" s="14">
+      <c r="Q21" s="14"/>
+      <c r="R21" s="13">
         <v>370189</v>
       </c>
-      <c r="S21" s="14">
+      <c r="S21" s="13">
         <v>19197</v>
       </c>
-      <c r="T21" s="14">
+      <c r="T21" s="13">
         <f t="shared" si="7"/>
         <v>389386</v>
       </c>
-      <c r="U21" s="49"/>
-      <c r="V21" s="24"/>
-      <c r="W21" s="43"/>
-      <c r="X21" s="25"/>
-      <c r="Y21" s="42"/>
-    </row>
-    <row r="22" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+      <c r="U21" s="56"/>
+      <c r="V21" s="23"/>
+      <c r="W21" s="3"/>
+      <c r="X21" s="24"/>
+    </row>
+    <row r="22" spans="1:24" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B22" s="23">
+      <c r="B22" s="22">
         <v>0.14149999999999999</v>
       </c>
-      <c r="C22" s="22"/>
-      <c r="D22" s="21">
+      <c r="C22" s="21"/>
+      <c r="D22" s="20">
         <v>6.4500000000000002E-2</v>
       </c>
-      <c r="E22" s="20"/>
-      <c r="F22" s="19">
+      <c r="E22" s="19"/>
+      <c r="F22" s="18">
         <v>0.74</v>
       </c>
-      <c r="G22" s="19">
+      <c r="G22" s="18">
         <v>0.26</v>
       </c>
-      <c r="H22" s="16">
+      <c r="H22" s="15">
         <f t="shared" si="0"/>
         <v>107050.06</v>
       </c>
-      <c r="I22" s="16">
+      <c r="I22" s="15">
         <f t="shared" si="1"/>
         <v>10186.800000000003</v>
       </c>
-      <c r="J22" s="16">
+      <c r="J22" s="15">
         <f t="shared" si="2"/>
         <v>304680.94</v>
       </c>
-      <c r="K22" s="16">
+      <c r="K22" s="15">
         <f t="shared" si="3"/>
         <v>28993.200000000012</v>
       </c>
-      <c r="L22" s="18">
+      <c r="L22" s="17">
         <f t="shared" si="4"/>
         <v>8.6890761147987078E-2</v>
       </c>
-      <c r="M22" s="17">
+      <c r="M22" s="16">
         <f t="shared" si="5"/>
         <v>0.11221835332762442</v>
       </c>
-      <c r="N22" s="17">
+      <c r="N22" s="16">
         <f t="shared" si="6"/>
         <v>0.11221835332762464</v>
       </c>
-      <c r="O22" s="16">
+      <c r="O22" s="15">
         <f t="shared" si="8"/>
         <v>756537.52650176687</v>
       </c>
-      <c r="P22" s="16">
+      <c r="P22" s="15">
         <f t="shared" si="9"/>
         <v>4723735.503875969</v>
       </c>
-      <c r="Q22" s="15"/>
-      <c r="R22" s="14">
+      <c r="Q22" s="14"/>
+      <c r="R22" s="13">
         <v>411731</v>
       </c>
-      <c r="S22" s="14">
+      <c r="S22" s="13">
         <v>39180</v>
       </c>
-      <c r="T22" s="14">
+      <c r="T22" s="13">
         <f t="shared" si="7"/>
         <v>450911</v>
       </c>
-      <c r="U22" s="49"/>
-      <c r="V22" s="42"/>
-      <c r="W22" s="42"/>
-      <c r="X22" s="25"/>
-      <c r="Y22" s="42"/>
-    </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="U22" s="56"/>
+      <c r="X22" s="24"/>
+    </row>
+    <row r="23" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A23" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B23" s="23">
+      <c r="B23" s="22">
         <v>0.14149999999999999</v>
       </c>
-      <c r="C23" s="22"/>
-      <c r="D23" s="21">
+      <c r="C23" s="21"/>
+      <c r="D23" s="20">
         <v>6.4299999999999996E-2</v>
       </c>
-      <c r="E23" s="20"/>
-      <c r="F23" s="19">
+      <c r="E23" s="19"/>
+      <c r="F23" s="18">
         <v>0.74</v>
       </c>
-      <c r="G23" s="19">
+      <c r="G23" s="18">
         <v>0.26</v>
       </c>
-      <c r="H23" s="16">
+      <c r="H23" s="15">
         <f t="shared" si="0"/>
         <v>109477.16</v>
       </c>
-      <c r="I23" s="16">
+      <c r="I23" s="15">
         <f t="shared" si="1"/>
         <v>10553.140000000014</v>
       </c>
-      <c r="J23" s="16">
+      <c r="J23" s="15">
         <f t="shared" si="2"/>
         <v>311588.83999999997</v>
       </c>
-      <c r="K23" s="16">
+      <c r="K23" s="15">
         <f t="shared" si="3"/>
         <v>30035.860000000044</v>
       </c>
-      <c r="L23" s="18">
+      <c r="L23" s="17">
         <f t="shared" si="4"/>
         <v>8.7920633373406554E-2</v>
       </c>
-      <c r="M23" s="17">
+      <c r="M23" s="16">
         <f t="shared" si="5"/>
         <v>2.2672570197531883E-2</v>
       </c>
-      <c r="N23" s="17">
+      <c r="N23" s="16">
         <f t="shared" si="6"/>
         <v>2.5853511317897482E-2</v>
       </c>
-      <c r="O23" s="16">
+      <c r="O23" s="15">
         <f t="shared" si="8"/>
         <v>773690.17667844531</v>
       </c>
-      <c r="P23" s="16">
+      <c r="P23" s="15">
         <f t="shared" si="9"/>
         <v>4845860.6531881802</v>
       </c>
-      <c r="Q23" s="15"/>
-      <c r="R23" s="14">
+      <c r="Q23" s="14"/>
+      <c r="R23" s="13">
         <v>421066</v>
       </c>
-      <c r="S23" s="14">
+      <c r="S23" s="13">
         <v>40589</v>
       </c>
-      <c r="T23" s="14">
+      <c r="T23" s="13">
         <f t="shared" si="7"/>
         <v>461655</v>
       </c>
-      <c r="U23" s="49"/>
-      <c r="V23" s="24"/>
-      <c r="W23" s="43"/>
-      <c r="X23" s="42"/>
-      <c r="Y23" s="42"/>
-    </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="U23" s="56"/>
+      <c r="V23" s="23"/>
+      <c r="W23" s="3"/>
+    </row>
+    <row r="24" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A24" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B24" s="23">
+      <c r="B24" s="22">
         <v>0.14149999999999999</v>
       </c>
-      <c r="C24" s="22"/>
-      <c r="D24" s="21">
+      <c r="C24" s="21"/>
+      <c r="D24" s="20">
         <v>6.4100000000000004E-2</v>
       </c>
-      <c r="E24" s="20"/>
-      <c r="F24" s="19">
+      <c r="E24" s="19"/>
+      <c r="F24" s="18">
         <v>0.74</v>
       </c>
-      <c r="G24" s="19">
+      <c r="G24" s="18">
         <v>0.26</v>
       </c>
-      <c r="H24" s="16">
+      <c r="H24" s="15">
         <f t="shared" si="0"/>
         <v>104551.46</v>
       </c>
-      <c r="I24" s="16">
+      <c r="I24" s="15">
         <f t="shared" si="1"/>
         <v>9389.64</v>
       </c>
-      <c r="J24" s="16">
+      <c r="J24" s="15">
         <f t="shared" si="2"/>
         <v>297569.53999999998</v>
       </c>
-      <c r="K24" s="16">
+      <c r="K24" s="15">
         <f t="shared" si="3"/>
         <v>26724.359999999986</v>
       </c>
-      <c r="L24" s="18">
+      <c r="L24" s="17">
         <f t="shared" si="4"/>
         <v>8.2407840542174857E-2</v>
       </c>
-      <c r="M24" s="17">
+      <c r="M24" s="16">
         <f t="shared" si="5"/>
         <v>-4.4992946473949358E-2</v>
       </c>
-      <c r="N24" s="17">
+      <c r="N24" s="16">
         <f t="shared" si="6"/>
         <v>-4.2013205277300347E-2</v>
       </c>
-      <c r="O24" s="16">
+      <c r="O24" s="15">
         <f t="shared" si="8"/>
         <v>738879.57597173157</v>
       </c>
-      <c r="P24" s="16">
+      <c r="P24" s="15">
         <f t="shared" si="9"/>
         <v>4642270.5148205925</v>
       </c>
-      <c r="Q24" s="15"/>
-      <c r="R24" s="14">
+      <c r="Q24" s="14"/>
+      <c r="R24" s="13">
         <v>402121</v>
       </c>
-      <c r="S24" s="14">
+      <c r="S24" s="13">
         <v>36114</v>
       </c>
-      <c r="T24" s="14">
+      <c r="T24" s="13">
         <f t="shared" si="7"/>
         <v>438235</v>
       </c>
-      <c r="U24" s="49"/>
-      <c r="V24" s="42"/>
-      <c r="W24" s="42"/>
-      <c r="X24" s="42"/>
-      <c r="Y24" s="42"/>
-    </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="U24" s="56"/>
+    </row>
+    <row r="25" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A25" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B25" s="23">
+      <c r="B25" s="22">
         <v>0.14149999999999999</v>
       </c>
-      <c r="C25" s="22"/>
-      <c r="D25" s="21">
+      <c r="C25" s="21"/>
+      <c r="D25" s="20">
         <v>6.3899999999999998E-2</v>
       </c>
-      <c r="E25" s="20"/>
-      <c r="F25" s="19">
+      <c r="E25" s="19"/>
+      <c r="F25" s="18">
         <v>0.74</v>
       </c>
-      <c r="G25" s="19">
+      <c r="G25" s="18">
         <v>0.26</v>
       </c>
-      <c r="H25" s="16">
+      <c r="H25" s="15">
         <f t="shared" si="0"/>
         <v>111054.84000000001</v>
       </c>
-      <c r="I25" s="16">
+      <c r="I25" s="15">
         <f t="shared" si="1"/>
         <v>12229.62000000001</v>
       </c>
-      <c r="J25" s="16">
+      <c r="J25" s="15">
         <f t="shared" si="2"/>
         <v>316079.15999999997</v>
       </c>
-      <c r="K25" s="16">
+      <c r="K25" s="15">
         <f t="shared" si="3"/>
         <v>34807.380000000005</v>
       </c>
-      <c r="L25" s="18">
+      <c r="L25" s="17">
         <f t="shared" si="4"/>
         <v>9.919839045407669E-2</v>
       </c>
-      <c r="M25" s="17">
+      <c r="M25" s="16">
         <f t="shared" si="5"/>
         <v>6.2202670340519406E-2</v>
       </c>
-      <c r="N25" s="17">
+      <c r="N25" s="16">
         <f t="shared" si="6"/>
         <v>6.5527248338455246E-2</v>
       </c>
-      <c r="O25" s="16">
+      <c r="O25" s="15">
         <f t="shared" si="8"/>
         <v>784839.85865724401</v>
       </c>
-      <c r="P25" s="16">
+      <c r="P25" s="15">
         <f t="shared" si="9"/>
         <v>4946465.7276995303</v>
       </c>
-      <c r="Q25" s="15"/>
-      <c r="R25" s="14">
+      <c r="Q25" s="14"/>
+      <c r="R25" s="13">
         <v>427134</v>
       </c>
-      <c r="S25" s="14">
+      <c r="S25" s="13">
         <v>47037</v>
       </c>
-      <c r="T25" s="14">
+      <c r="T25" s="13">
         <f t="shared" si="7"/>
         <v>474171</v>
       </c>
-      <c r="U25" s="49"/>
-      <c r="V25" s="24"/>
-      <c r="W25" s="43"/>
-      <c r="X25" s="42"/>
-      <c r="Y25" s="42"/>
-    </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="U25" s="56"/>
+      <c r="V25" s="23"/>
+      <c r="W25" s="3"/>
+    </row>
+    <row r="26" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A26" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B26" s="23">
+      <c r="B26" s="22">
         <v>0.14149999999999999</v>
       </c>
-      <c r="C26" s="22"/>
-      <c r="D26" s="21">
+      <c r="C26" s="21"/>
+      <c r="D26" s="20">
         <v>6.3500000000000001E-2</v>
       </c>
-      <c r="E26" s="20"/>
-      <c r="F26" s="19">
+      <c r="E26" s="19"/>
+      <c r="F26" s="18">
         <v>0.73</v>
       </c>
-      <c r="G26" s="19">
+      <c r="G26" s="18">
         <v>0.27</v>
       </c>
-      <c r="H26" s="16">
+      <c r="H26" s="15">
         <f t="shared" si="0"/>
         <v>107091.45000000001</v>
       </c>
-      <c r="I26" s="16">
+      <c r="I26" s="15">
         <f t="shared" si="1"/>
         <v>5640.5699999999924</v>
       </c>
-      <c r="J26" s="16">
+      <c r="J26" s="15">
         <f t="shared" si="2"/>
         <v>289543.55</v>
       </c>
-      <c r="K26" s="16">
+      <c r="K26" s="15">
         <f t="shared" si="3"/>
         <v>15250.429999999993</v>
       </c>
-      <c r="L26" s="18">
+      <c r="L26" s="17">
         <f t="shared" si="4"/>
         <v>5.0035207388282404E-2</v>
       </c>
-      <c r="M26" s="17">
+      <c r="M26" s="16">
         <f t="shared" si="5"/>
         <v>-3.5688584126545075E-2</v>
       </c>
-      <c r="N26" s="17">
+      <c r="N26" s="16">
         <f t="shared" si="6"/>
         <v>-7.8182040290309618E-2</v>
       </c>
-      <c r="O26" s="16">
+      <c r="O26" s="15">
         <f t="shared" si="8"/>
         <v>756830.0353356892</v>
       </c>
-      <c r="P26" s="16">
+      <c r="P26" s="15">
         <f t="shared" si="9"/>
         <v>4559740.94488189</v>
       </c>
-      <c r="Q26" s="15"/>
-      <c r="R26" s="14">
+      <c r="Q26" s="14"/>
+      <c r="R26" s="13">
         <v>396635</v>
       </c>
-      <c r="S26" s="14">
+      <c r="S26" s="13">
         <v>20891</v>
       </c>
-      <c r="T26" s="14">
+      <c r="T26" s="13">
         <f t="shared" si="7"/>
         <v>417526</v>
       </c>
-      <c r="U26" s="49"/>
-      <c r="V26" s="24"/>
-      <c r="W26" s="43"/>
-      <c r="X26" s="42"/>
-      <c r="Y26" s="42"/>
-    </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="U26" s="56"/>
+      <c r="V26" s="23"/>
+      <c r="W26" s="3"/>
+    </row>
+    <row r="27" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A27" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="23">
+      <c r="B27" s="22">
         <v>0.14149999999999999</v>
       </c>
-      <c r="C27" s="22"/>
-      <c r="D27" s="21">
+      <c r="C27" s="21"/>
+      <c r="D27" s="20">
         <v>6.3E-2</v>
       </c>
-      <c r="E27" s="20"/>
-      <c r="F27" s="19">
+      <c r="E27" s="19"/>
+      <c r="F27" s="18">
         <v>0.73</v>
       </c>
-      <c r="G27" s="19">
+      <c r="G27" s="18">
         <v>0.27</v>
       </c>
-      <c r="H27" s="16">
+      <c r="H27" s="15">
         <f t="shared" si="0"/>
         <v>115792.47</v>
       </c>
-      <c r="I27" s="16">
+      <c r="I27" s="15">
         <f t="shared" si="1"/>
         <v>4646.6999999999971</v>
       </c>
-      <c r="J27" s="16">
+      <c r="J27" s="15">
         <f t="shared" si="2"/>
         <v>313068.52999999997</v>
       </c>
-      <c r="K27" s="16">
+      <c r="K27" s="15">
         <f t="shared" si="3"/>
         <v>12563.299999999988</v>
       </c>
-      <c r="L27" s="18">
+      <c r="L27" s="17">
         <f t="shared" si="4"/>
         <v>3.8581302079713768E-2</v>
       </c>
-      <c r="M27" s="17">
+      <c r="M27" s="16">
         <f t="shared" si="5"/>
         <v>8.124850303175446E-2</v>
       </c>
-      <c r="N27" s="17">
+      <c r="N27" s="16">
         <f t="shared" si="6"/>
         <v>8.9829840357403379E-2</v>
       </c>
-      <c r="O27" s="16">
+      <c r="O27" s="15">
         <f t="shared" si="8"/>
         <v>818321.34275618382</v>
       </c>
-      <c r="P27" s="16">
+      <c r="P27" s="15">
         <f t="shared" si="9"/>
         <v>4969341.7460317453</v>
       </c>
-      <c r="Q27" s="15"/>
-      <c r="R27" s="14">
+      <c r="Q27" s="14"/>
+      <c r="R27" s="13">
         <v>428861</v>
       </c>
-      <c r="S27" s="14">
+      <c r="S27" s="13">
         <v>17210</v>
       </c>
-      <c r="T27" s="14">
+      <c r="T27" s="13">
         <f t="shared" si="7"/>
         <v>446071</v>
       </c>
-      <c r="U27" s="49"/>
-      <c r="V27" s="24"/>
-      <c r="W27" s="43"/>
-      <c r="X27" s="42"/>
-      <c r="Y27" s="42"/>
-    </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="U27" s="56"/>
+      <c r="V27" s="23"/>
+      <c r="W27" s="3"/>
+    </row>
+    <row r="28" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A28" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B28" s="23">
+      <c r="B28" s="22">
         <v>0.14149999999999999</v>
       </c>
-      <c r="C28" s="22"/>
-      <c r="D28" s="21">
+      <c r="C28" s="21"/>
+      <c r="D28" s="20">
         <v>6.25E-2</v>
       </c>
-      <c r="E28" s="20"/>
-      <c r="F28" s="19">
+      <c r="E28" s="19"/>
+      <c r="F28" s="18">
         <v>0.73</v>
       </c>
-      <c r="G28" s="19">
+      <c r="G28" s="18">
         <v>0.27</v>
       </c>
-      <c r="H28" s="16">
+      <c r="H28" s="15">
         <f t="shared" si="0"/>
         <v>136796.58000000002</v>
       </c>
-      <c r="I28" s="16">
+      <c r="I28" s="15">
         <f t="shared" si="1"/>
         <v>9239.3999999999942</v>
       </c>
-      <c r="J28" s="16">
+      <c r="J28" s="15">
         <f t="shared" si="2"/>
         <v>369857.42</v>
       </c>
-      <c r="K28" s="16">
+      <c r="K28" s="15">
         <f t="shared" si="3"/>
         <v>24980.600000000035</v>
       </c>
-      <c r="L28" s="18">
+      <c r="L28" s="17">
         <f t="shared" si="4"/>
         <v>6.3267969989313597E-2</v>
       </c>
-      <c r="M28" s="17">
+      <c r="M28" s="16">
         <f t="shared" si="5"/>
         <v>0.1813944378248431</v>
       </c>
-      <c r="N28" s="17">
+      <c r="N28" s="16">
         <f t="shared" si="6"/>
         <v>0.19084559332744178</v>
       </c>
-      <c r="O28" s="16">
+      <c r="O28" s="15">
         <f t="shared" si="8"/>
         <v>966760.28268551256</v>
       </c>
-      <c r="P28" s="16">
+      <c r="P28" s="15">
         <f t="shared" si="9"/>
         <v>5917718.7199999997</v>
       </c>
-      <c r="Q28" s="15"/>
-      <c r="R28" s="40">
+      <c r="Q28" s="14"/>
+      <c r="R28" s="13">
         <v>506654</v>
       </c>
-      <c r="S28" s="40">
+      <c r="S28" s="13">
         <v>34220</v>
       </c>
-      <c r="T28" s="14">
+      <c r="T28" s="13">
         <f t="shared" si="7"/>
         <v>540874</v>
       </c>
-      <c r="U28" s="49"/>
-      <c r="V28" s="24"/>
-      <c r="W28" s="43"/>
-      <c r="X28" s="42"/>
-      <c r="Y28" s="42"/>
-    </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="U28" s="56"/>
+      <c r="V28" s="23"/>
+      <c r="W28" s="3"/>
+    </row>
+    <row r="29" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A29" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="23">
+      <c r="B29" s="22">
         <v>0.14149999999999999</v>
       </c>
-      <c r="C29" s="22"/>
-      <c r="D29" s="21">
+      <c r="C29" s="21"/>
+      <c r="D29" s="20">
         <v>6.2E-2</v>
       </c>
-      <c r="E29" s="20"/>
-      <c r="F29" s="19">
+      <c r="E29" s="19"/>
+      <c r="F29" s="18">
         <v>0.73</v>
       </c>
-      <c r="G29" s="19">
+      <c r="G29" s="18">
         <v>0.27</v>
       </c>
-      <c r="H29" s="16">
+      <c r="H29" s="15">
         <f t="shared" si="0"/>
         <v>133619.76</v>
       </c>
-      <c r="I29" s="16">
+      <c r="I29" s="15">
         <f t="shared" si="1"/>
         <v>10624.76999999999</v>
       </c>
-      <c r="J29" s="16">
+      <c r="J29" s="15">
         <f t="shared" si="2"/>
         <v>361268.24</v>
       </c>
-      <c r="K29" s="16">
+      <c r="K29" s="15">
         <f t="shared" si="3"/>
         <v>28726.229999999981</v>
       </c>
-      <c r="L29" s="18">
+      <c r="L29" s="17">
         <f t="shared" si="4"/>
         <v>7.365804443329671E-2</v>
       </c>
-      <c r="M29" s="17">
+      <c r="M29" s="16">
         <f t="shared" si="5"/>
         <v>-2.3222948994777615E-2</v>
       </c>
-      <c r="N29" s="17">
+      <c r="N29" s="16">
         <f t="shared" si="6"/>
         <v>-1.5345714712477254E-2</v>
       </c>
-      <c r="O29" s="16">
+      <c r="O29" s="15">
         <f t="shared" si="8"/>
         <v>944309.25795053015</v>
       </c>
-      <c r="P29" s="16">
+      <c r="P29" s="15">
         <f t="shared" si="9"/>
         <v>5826907.0967741935</v>
       </c>
-      <c r="Q29" s="15"/>
-      <c r="R29" s="45">
+      <c r="Q29" s="14"/>
+      <c r="R29" s="13">
         <f>225683+269205</f>
         <v>494888</v>
       </c>
-      <c r="S29" s="45">
+      <c r="S29" s="13">
         <v>39351</v>
       </c>
-      <c r="T29" s="14">
+      <c r="T29" s="13">
         <f t="shared" si="7"/>
         <v>534239</v>
       </c>
-      <c r="U29" s="49"/>
-      <c r="V29" s="24"/>
-      <c r="W29" s="43"/>
-      <c r="X29" s="42"/>
-      <c r="Y29" s="42"/>
-    </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.15">
-      <c r="A30" s="51" t="s">
+      <c r="U29" s="56"/>
+      <c r="V29" s="23"/>
+      <c r="W29" s="3"/>
+    </row>
+    <row r="30" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="A30" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B30" s="52">
+      <c r="B30" s="22">
         <v>0.14149999999999999</v>
       </c>
-      <c r="C30" s="53"/>
-      <c r="D30" s="54">
+      <c r="C30" s="8"/>
+      <c r="D30" s="20">
         <v>6.2E-2</v>
       </c>
-      <c r="E30" s="54"/>
-      <c r="F30" s="55">
+      <c r="E30" s="20"/>
+      <c r="F30" s="18">
         <v>0.73</v>
       </c>
-      <c r="G30" s="55">
+      <c r="G30" s="18">
         <v>0.27</v>
       </c>
-      <c r="H30" s="56">
+      <c r="H30" s="41">
         <v>131613.39000000001</v>
       </c>
-      <c r="I30" s="57">
+      <c r="I30" s="15">
         <v>14618.339999999997</v>
       </c>
-      <c r="J30" s="57">
+      <c r="J30" s="15">
         <v>355843.61</v>
       </c>
-      <c r="K30" s="57">
+      <c r="K30" s="15">
         <v>39523.659999999974</v>
       </c>
-      <c r="L30" s="58">
+      <c r="L30" s="42">
         <v>9.9966949717410852E-2</v>
       </c>
-      <c r="M30" s="59">
+      <c r="M30" s="16">
         <v>-1.501551866280848E-2</v>
       </c>
-      <c r="N30" s="59">
+      <c r="N30" s="16">
         <v>-1.5015518662808591E-2</v>
       </c>
-      <c r="O30" s="57">
+      <c r="O30" s="15">
         <v>930129.96466431115</v>
       </c>
-      <c r="P30" s="57">
+      <c r="P30" s="15">
         <v>5739413.064516129</v>
       </c>
-      <c r="Q30" s="60"/>
-      <c r="R30" s="45">
+      <c r="Q30" s="52"/>
+      <c r="R30" s="13">
         <v>487457</v>
       </c>
-      <c r="S30" s="45">
+      <c r="S30" s="13">
         <v>54142</v>
       </c>
-      <c r="T30" s="61">
+      <c r="T30" s="13">
         <v>541599</v>
       </c>
-      <c r="U30" s="46"/>
-      <c r="V30" s="42"/>
-      <c r="W30" s="42"/>
-      <c r="X30" s="42"/>
-      <c r="Y30" s="42"/>
-    </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.15">
-      <c r="A31" s="12"/>
-      <c r="B31" s="5"/>
-      <c r="D31" s="6"/>
-      <c r="F31" s="10"/>
-      <c r="G31" s="10"/>
-      <c r="H31" s="9"/>
-      <c r="I31" s="3"/>
-      <c r="J31" s="3"/>
-      <c r="K31" s="3"/>
-      <c r="L31" s="3"/>
-      <c r="M31" s="4"/>
-      <c r="N31" s="4"/>
-      <c r="O31" s="13"/>
-      <c r="P31" s="13"/>
-      <c r="T31" s="3"/>
-      <c r="U31" s="50"/>
-      <c r="V31" s="42"/>
-      <c r="W31" s="42"/>
-      <c r="X31" s="42"/>
-      <c r="Y31" s="42"/>
-    </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="U30" s="56"/>
+    </row>
+    <row r="31" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="A31" s="43" t="s">
+        <v>48</v>
+      </c>
+      <c r="B31" s="44">
+        <v>0.14149999999999999</v>
+      </c>
+      <c r="C31" s="45"/>
+      <c r="D31" s="46">
+        <v>6.2E-2</v>
+      </c>
+      <c r="E31" s="47"/>
+      <c r="F31" s="48">
+        <v>0.78200000000000003</v>
+      </c>
+      <c r="G31" s="48">
+        <v>0.218</v>
+      </c>
+      <c r="H31" s="49">
+        <f>G31*R31</f>
+        <v>158524.15</v>
+      </c>
+      <c r="I31" s="49">
+        <f t="shared" ref="I31" si="10">(H31/(1-$L31))-H31</f>
+        <v>4946.4200000000128</v>
+      </c>
+      <c r="J31" s="49">
+        <f>F31*R31</f>
+        <v>568650.85</v>
+      </c>
+      <c r="K31" s="49">
+        <f t="shared" ref="K31" si="11">(J31/(1-$L31))-J31</f>
+        <v>17743.580000000075</v>
+      </c>
+      <c r="L31" s="50">
+        <f>S31/(R31+S31)</f>
+        <v>3.0258779913717802E-2</v>
+      </c>
+      <c r="M31" s="51">
+        <f>(O31/O30)-1</f>
+        <v>0.20446825357207188</v>
+      </c>
+      <c r="N31" s="51">
+        <f>(P31/P30)-1</f>
+        <v>0.59803586187763758</v>
+      </c>
+      <c r="O31" s="49">
+        <f>H31/B31</f>
+        <v>1120312.0141342757</v>
+      </c>
+      <c r="P31" s="49">
+        <f>J31/D31</f>
+        <v>9171787.9032258056</v>
+      </c>
+      <c r="Q31" s="52"/>
+      <c r="R31" s="53">
+        <f>723606+3570-1</f>
+        <v>727175</v>
+      </c>
+      <c r="S31" s="53">
+        <v>22690</v>
+      </c>
+      <c r="T31" s="53">
+        <f>R31+S31</f>
+        <v>749865</v>
+      </c>
+      <c r="U31" s="57"/>
+    </row>
+    <row r="32" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A32" s="4"/>
       <c r="B32" s="5"/>
       <c r="C32" s="3"/>
@@ -3490,13 +3503,8 @@
       <c r="R32" s="3"/>
       <c r="S32" s="3"/>
       <c r="T32" s="3"/>
-      <c r="U32" s="42"/>
-      <c r="V32" s="42"/>
-      <c r="W32" s="42"/>
-      <c r="X32" s="42"/>
-      <c r="Y32" s="42"/>
-    </row>
-    <row r="33" spans="1:25" x14ac:dyDescent="0.15">
+    </row>
+    <row r="33" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A33" s="4"/>
       <c r="B33" s="5"/>
       <c r="C33" s="3"/>
@@ -3517,13 +3525,9 @@
       <c r="R33" s="3"/>
       <c r="S33" s="3"/>
       <c r="T33" s="3"/>
-      <c r="U33" s="43"/>
-      <c r="V33" s="42"/>
-      <c r="W33" s="42"/>
-      <c r="X33" s="42"/>
-      <c r="Y33" s="42"/>
-    </row>
-    <row r="34" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="U33" s="3"/>
+    </row>
+    <row r="34" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A34" s="3"/>
       <c r="B34" s="5"/>
       <c r="C34" s="3"/>
@@ -3542,13 +3546,9 @@
       <c r="R34" s="3"/>
       <c r="S34" s="3"/>
       <c r="T34" s="3"/>
-      <c r="U34" s="43"/>
-      <c r="V34" s="42"/>
-      <c r="W34" s="42"/>
-      <c r="X34" s="42"/>
-      <c r="Y34" s="42"/>
-    </row>
-    <row r="35" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="U34" s="3"/>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
@@ -3569,13 +3569,9 @@
       <c r="R35" s="3"/>
       <c r="S35" s="3"/>
       <c r="T35" s="3"/>
-      <c r="U35" s="43"/>
-      <c r="V35" s="42"/>
-      <c r="W35" s="42"/>
-      <c r="X35" s="42"/>
-      <c r="Y35" s="42"/>
-    </row>
-    <row r="36" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="U35" s="3"/>
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
@@ -3596,13 +3592,9 @@
       <c r="R36" s="3"/>
       <c r="S36" s="3"/>
       <c r="T36" s="3"/>
-      <c r="U36" s="43"/>
-      <c r="V36" s="42"/>
-      <c r="W36" s="42"/>
-      <c r="X36" s="42"/>
-      <c r="Y36" s="42"/>
-    </row>
-    <row r="37" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="U36" s="3"/>
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
@@ -3623,13 +3615,9 @@
       <c r="R37" s="3"/>
       <c r="S37" s="3"/>
       <c r="T37" s="3"/>
-      <c r="U37" s="43"/>
-      <c r="V37" s="42"/>
-      <c r="W37" s="42"/>
-      <c r="X37" s="42"/>
-      <c r="Y37" s="42"/>
-    </row>
-    <row r="38" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="U37" s="3"/>
+    </row>
+    <row r="38" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A38" s="3"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
@@ -3650,13 +3638,9 @@
       <c r="R38" s="3"/>
       <c r="S38" s="3"/>
       <c r="T38" s="3"/>
-      <c r="U38" s="43"/>
-      <c r="V38" s="42"/>
-      <c r="W38" s="42"/>
-      <c r="X38" s="42"/>
-      <c r="Y38" s="42"/>
-    </row>
-    <row r="39" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="U38" s="3"/>
+    </row>
+    <row r="39" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A39" s="3"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
@@ -3677,13 +3661,9 @@
       <c r="R39" s="3"/>
       <c r="S39" s="3"/>
       <c r="T39" s="3"/>
-      <c r="U39" s="43"/>
-      <c r="V39" s="42"/>
-      <c r="W39" s="42"/>
-      <c r="X39" s="42"/>
-      <c r="Y39" s="42"/>
-    </row>
-    <row r="40" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="U39" s="3"/>
+    </row>
+    <row r="40" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
@@ -3704,13 +3684,9 @@
       <c r="R40" s="3"/>
       <c r="S40" s="3"/>
       <c r="T40" s="3"/>
-      <c r="U40" s="43"/>
-      <c r="V40" s="42"/>
-      <c r="W40" s="42"/>
-      <c r="X40" s="42"/>
-      <c r="Y40" s="42"/>
-    </row>
-    <row r="41" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="U40" s="3"/>
+    </row>
+    <row r="41" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A41" s="3"/>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
@@ -3731,13 +3707,9 @@
       <c r="R41" s="3"/>
       <c r="S41" s="3"/>
       <c r="T41" s="3"/>
-      <c r="U41" s="43"/>
-      <c r="V41" s="42"/>
-      <c r="W41" s="42"/>
-      <c r="X41" s="42"/>
-      <c r="Y41" s="42"/>
-    </row>
-    <row r="42" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="U41" s="3"/>
+    </row>
+    <row r="42" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A42" s="3"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
@@ -3758,13 +3730,9 @@
       <c r="R42" s="3"/>
       <c r="S42" s="3"/>
       <c r="T42" s="3"/>
-      <c r="U42" s="43"/>
-      <c r="V42" s="42"/>
-      <c r="W42" s="42"/>
-      <c r="X42" s="42"/>
-      <c r="Y42" s="42"/>
-    </row>
-    <row r="43" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="U42" s="3"/>
+    </row>
+    <row r="43" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A43" s="3"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
@@ -3785,13 +3753,9 @@
       <c r="R43" s="3"/>
       <c r="S43" s="3"/>
       <c r="T43" s="3"/>
-      <c r="U43" s="43"/>
-      <c r="V43" s="42"/>
-      <c r="W43" s="42"/>
-      <c r="X43" s="42"/>
-      <c r="Y43" s="42"/>
-    </row>
-    <row r="44" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="U43" s="3"/>
+    </row>
+    <row r="44" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A44" s="3"/>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
@@ -3812,13 +3776,9 @@
       <c r="R44" s="3"/>
       <c r="S44" s="3"/>
       <c r="T44" s="3"/>
-      <c r="U44" s="43"/>
-      <c r="V44" s="42"/>
-      <c r="W44" s="42"/>
-      <c r="X44" s="42"/>
-      <c r="Y44" s="42"/>
-    </row>
-    <row r="45" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="U44" s="3"/>
+    </row>
+    <row r="45" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A45" s="3"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
@@ -3839,13 +3799,9 @@
       <c r="R45" s="3"/>
       <c r="S45" s="3"/>
       <c r="T45" s="3"/>
-      <c r="U45" s="43"/>
-      <c r="V45" s="42"/>
-      <c r="W45" s="42"/>
-      <c r="X45" s="42"/>
-      <c r="Y45" s="42"/>
-    </row>
-    <row r="46" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="U45" s="3"/>
+    </row>
+    <row r="46" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A46" s="3"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
@@ -3866,13 +3822,9 @@
       <c r="R46" s="3"/>
       <c r="S46" s="3"/>
       <c r="T46" s="3"/>
-      <c r="U46" s="43"/>
-      <c r="V46" s="42"/>
-      <c r="W46" s="42"/>
-      <c r="X46" s="42"/>
-      <c r="Y46" s="42"/>
-    </row>
-    <row r="47" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="U46" s="3"/>
+    </row>
+    <row r="47" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A47" s="3"/>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
@@ -3893,9 +3845,9 @@
       <c r="R47" s="3"/>
       <c r="S47" s="3"/>
       <c r="T47" s="3"/>
-      <c r="U47" s="43"/>
-    </row>
-    <row r="48" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="U47" s="3"/>
+    </row>
+    <row r="48" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A48" s="3"/>
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
@@ -5603,7 +5555,7 @@
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="U3:W3"/>
-    <mergeCell ref="U4:U29"/>
+    <mergeCell ref="U4:U31"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.5" bottom="0.25" header="0.25" footer="0.25"/>
   <pageSetup scale="55" orientation="landscape" r:id="rId1"/>

</xml_diff>